<commit_message>
feat: implement print_completion and fix MTPO
</commit_message>
<xml_diff>
--- a/SMCR.xlsx
+++ b/SMCR.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="40">
   <si>
     <t>Method</t>
   </si>
@@ -120,6 +120,12 @@
   </si>
   <si>
     <t>SMCR-brier-scale-weight</t>
+  </si>
+  <si>
+    <t>SMCR-only-brier</t>
+  </si>
+  <si>
+    <t>SMCR-only-brier-std</t>
   </si>
   <si>
     <t>SMCR-ECE</t>
@@ -1374,17 +1380,17 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:AK56"/>
+  <dimension ref="A1:AK58"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection/>
-      <selection pane="topRight" activeCell="K26" sqref="K26"/>
+      <selection pane="topRight" activeCell="B46" sqref="B46:AG48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14" defaultRowHeight="15.2"/>
   <cols>
-    <col min="1" max="1" width="22.1538461538462" style="1" customWidth="1"/>
+    <col min="1" max="1" width="24.5096153846154" style="1" customWidth="1"/>
     <col min="2" max="8" width="14" style="1"/>
     <col min="9" max="33" width="14" style="1" customWidth="1"/>
     <col min="34" max="16384" width="14" style="1"/>
@@ -1829,19 +1835,19 @@
       <c r="AF7" s="20"/>
       <c r="AG7" s="20"/>
       <c r="AH7" s="22" t="e">
-        <f t="shared" ref="AH7:AH18" si="1">AVERAGE(AD7,Z7,V7,R7,N7,J7,F7)</f>
+        <f t="shared" ref="AH7:AH17" si="1">AVERAGE(AD7,Z7,V7,R7,N7,J7,F7)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="AI7" s="22" t="e">
-        <f t="shared" ref="AI7:AI18" si="2">AVERAGE(AE7,AA7,W7,S7,O7,K7,G7)</f>
+        <f t="shared" ref="AI7:AI17" si="2">AVERAGE(AE7,AA7,W7,S7,O7,K7,G7)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="AJ7" s="22" t="e">
-        <f t="shared" ref="AJ7:AJ18" si="3">AVERAGE(AF7,AB7,X7,T7,P7,L7,H7)</f>
+        <f t="shared" ref="AJ7:AJ17" si="3">AVERAGE(AF7,AB7,X7,T7,P7,L7,H7)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="AK7" s="22" t="e">
-        <f t="shared" ref="AK7:AK18" si="4">AVERAGE(AG7,AC7,Y7,U7,Q7,M7,I7)</f>
+        <f t="shared" ref="AK7:AK17" si="4">AVERAGE(AG7,AC7,Y7,U7,Q7,M7,I7)</f>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -2384,20 +2390,20 @@
         <v>0.2325658</v>
       </c>
       <c r="AH14" s="22">
-        <f>AVERAGE(AD14,Z12,V14,R14,N14,J14,F14)</f>
-        <v>0.522928909571491</v>
+        <f t="shared" si="1"/>
+        <v>0.521954145139562</v>
       </c>
       <c r="AI14" s="22">
-        <f>AVERAGE(AE14,AA12,W14,S14,O14,K14,G14)</f>
-        <v>0.65470101428949</v>
+        <f t="shared" si="2"/>
+        <v>0.66796309801542</v>
       </c>
       <c r="AJ14" s="22">
-        <f>AVERAGE(AF14,AB12,X14,T14,P14,L14,H14)</f>
-        <v>0.2585196526721</v>
+        <f t="shared" si="3"/>
+        <v>0.256796790486713</v>
       </c>
       <c r="AK14" s="22">
-        <f>AVERAGE(AG14,AC12,Y14,U14,Q14,M14,I14)</f>
-        <v>0.239768638941366</v>
+        <f t="shared" si="4"/>
+        <v>0.23539992874426</v>
       </c>
     </row>
     <row r="15" ht="19" customHeight="1" spans="1:37">
@@ -2521,110 +2527,238 @@
       <c r="A16" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="B16" s="21"/>
-      <c r="C16" s="21"/>
-      <c r="D16" s="21"/>
-      <c r="E16" s="21"/>
-      <c r="F16" s="21"/>
-      <c r="G16" s="21"/>
-      <c r="H16" s="21"/>
-      <c r="I16" s="21"/>
-      <c r="J16" s="21"/>
-      <c r="K16" s="21"/>
-      <c r="L16" s="21"/>
-      <c r="M16" s="21"/>
-      <c r="N16" s="21"/>
-      <c r="O16" s="21"/>
-      <c r="P16" s="21"/>
-      <c r="Q16" s="21"/>
-      <c r="R16" s="21"/>
-      <c r="S16" s="21"/>
-      <c r="T16" s="21"/>
-      <c r="U16" s="21"/>
-      <c r="V16" s="21"/>
-      <c r="W16" s="21"/>
-      <c r="X16" s="21"/>
-      <c r="Y16" s="21"/>
-      <c r="Z16" s="21"/>
-      <c r="AA16" s="21"/>
-      <c r="AB16" s="21"/>
-      <c r="AC16" s="21"/>
-      <c r="AD16" s="21"/>
-      <c r="AE16" s="21"/>
-      <c r="AF16" s="21"/>
-      <c r="AG16" s="21"/>
-      <c r="AH16" s="22" t="e">
+      <c r="B16" s="20">
+        <v>0.486</v>
+      </c>
+      <c r="C16" s="20">
+        <v>0.644941634241245</v>
+      </c>
+      <c r="D16" s="20">
+        <v>0.242802499999999</v>
+      </c>
+      <c r="E16" s="20">
+        <v>0.09255</v>
+      </c>
+      <c r="F16" s="20">
+        <v>0.0862228386500231</v>
+      </c>
+      <c r="G16" s="20">
+        <v>0.686647871199733</v>
+      </c>
+      <c r="H16" s="20">
+        <v>0.126937702265372</v>
+      </c>
+      <c r="I16" s="20">
+        <v>0.16219371243643</v>
+      </c>
+      <c r="J16" s="20">
+        <v>0.466</v>
+      </c>
+      <c r="K16" s="20">
+        <v>0.754465146838983</v>
+      </c>
+      <c r="L16" s="20">
+        <v>0.200336249999999</v>
+      </c>
+      <c r="M16" s="20">
+        <v>0.0242749999999999</v>
+      </c>
+      <c r="N16" s="20">
+        <v>0.846846846846846</v>
+      </c>
+      <c r="O16" s="20">
+        <v>0.709882704620445</v>
+      </c>
+      <c r="P16" s="20">
+        <v>0.300735053235053</v>
+      </c>
+      <c r="Q16" s="20">
+        <v>0.423218673218673</v>
+      </c>
+      <c r="R16" s="20">
+        <v>0.419642857142857</v>
+      </c>
+      <c r="S16" s="20">
+        <v>0.534349427168576</v>
+      </c>
+      <c r="T16" s="20">
+        <v>0.259198875</v>
+      </c>
+      <c r="U16" s="20">
+        <v>0.115392857142857</v>
+      </c>
+      <c r="V16" s="20">
+        <v>0.484</v>
+      </c>
+      <c r="W16" s="20">
+        <v>0.693382023191748</v>
+      </c>
+      <c r="X16" s="20">
+        <v>0.229448446609876</v>
+      </c>
+      <c r="Y16" s="20">
+        <v>0.0940892444444445</v>
+      </c>
+      <c r="Z16" s="20">
+        <v>0.736921910538286</v>
+      </c>
+      <c r="AA16" s="20">
+        <v>0.628915098255476</v>
+      </c>
+      <c r="AB16" s="20">
+        <v>0.20057073540561</v>
+      </c>
+      <c r="AC16" s="20">
+        <v>0.118119787717968</v>
+      </c>
+      <c r="AD16" s="20">
+        <v>0.484</v>
+      </c>
+      <c r="AE16" s="20">
+        <v>0.693382023191748</v>
+      </c>
+      <c r="AF16" s="20">
+        <v>0.229448446609876</v>
+      </c>
+      <c r="AG16" s="20">
+        <v>0.0940892444444445</v>
+      </c>
+      <c r="AH16" s="22">
         <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="AI16" s="22" t="e">
+        <v>0.503376350454002</v>
+      </c>
+      <c r="AI16" s="22">
         <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="AJ16" s="22" t="e">
+        <v>0.67157489920953</v>
+      </c>
+      <c r="AJ16" s="22">
         <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="AK16" s="22" t="e">
+        <v>0.220953644160827</v>
+      </c>
+      <c r="AK16" s="22">
         <f t="shared" si="4"/>
-        <v>#DIV/0!</v>
+        <v>0.147339788486402</v>
       </c>
     </row>
     <row r="17" ht="19" customHeight="1" spans="1:37">
       <c r="A17" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="B17" s="21"/>
-      <c r="C17" s="21"/>
-      <c r="D17" s="21"/>
-      <c r="E17" s="21"/>
-      <c r="F17" s="21"/>
-      <c r="G17" s="21"/>
-      <c r="H17" s="21"/>
-      <c r="I17" s="21"/>
-      <c r="J17" s="21"/>
-      <c r="K17" s="21"/>
-      <c r="L17" s="21"/>
-      <c r="M17" s="21"/>
-      <c r="N17" s="21"/>
-      <c r="O17" s="21"/>
-      <c r="P17" s="21"/>
-      <c r="Q17" s="21"/>
-      <c r="R17" s="21"/>
-      <c r="S17" s="21"/>
-      <c r="T17" s="21"/>
-      <c r="U17" s="21"/>
-      <c r="V17" s="21"/>
-      <c r="W17" s="21"/>
-      <c r="X17" s="21"/>
-      <c r="Y17" s="21"/>
-      <c r="Z17" s="21"/>
-      <c r="AA17" s="21"/>
-      <c r="AB17" s="21"/>
-      <c r="AC17" s="21"/>
-      <c r="AD17" s="21"/>
-      <c r="AE17" s="21"/>
-      <c r="AF17" s="21"/>
-      <c r="AG17" s="21"/>
-      <c r="AH17" s="22" t="e">
+      <c r="B17" s="20">
+        <v>0.481</v>
+      </c>
+      <c r="C17" s="20">
+        <v>0.681429984898192</v>
+      </c>
+      <c r="D17" s="20">
+        <v>0.3126195</v>
+      </c>
+      <c r="E17" s="20">
+        <v>0.28549</v>
+      </c>
+      <c r="F17" s="20">
+        <v>0.0358298659269533</v>
+      </c>
+      <c r="G17" s="20">
+        <v>0.867401644225489</v>
+      </c>
+      <c r="H17" s="20">
+        <v>0.0428304905224225</v>
+      </c>
+      <c r="I17" s="20">
+        <v>0.0391095700416088</v>
+      </c>
+      <c r="J17" s="20">
+        <v>0.45</v>
+      </c>
+      <c r="K17" s="20">
+        <v>0.841053535353535</v>
+      </c>
+      <c r="L17" s="20">
+        <v>0.18677485</v>
+      </c>
+      <c r="M17" s="20">
+        <v>0.142215</v>
+      </c>
+      <c r="N17" s="20">
+        <v>0.864045864045864</v>
+      </c>
+      <c r="O17" s="20">
+        <v>0.700642379946325</v>
+      </c>
+      <c r="P17" s="20">
+        <v>0.300390008190008</v>
+      </c>
+      <c r="Q17" s="20">
+        <v>0.345520065520065</v>
+      </c>
+      <c r="R17" s="20">
+        <v>0.399553571428571</v>
+      </c>
+      <c r="S17" s="20">
+        <v>0.555440177774085</v>
+      </c>
+      <c r="T17" s="20">
+        <v>0.312605678571428</v>
+      </c>
+      <c r="U17" s="20">
+        <v>0.252205357142857</v>
+      </c>
+      <c r="V17" s="20">
+        <v>0.444</v>
+      </c>
+      <c r="W17" s="20">
+        <v>0.760094627001101</v>
+      </c>
+      <c r="X17" s="20">
+        <v>0.2376051007</v>
+      </c>
+      <c r="Y17" s="20">
+        <v>0.2070482</v>
+      </c>
+      <c r="Z17" s="20">
+        <v>0.743745261561789</v>
+      </c>
+      <c r="AA17" s="20">
+        <v>0.695020477836286</v>
+      </c>
+      <c r="AB17" s="20">
+        <v>0.189060279853439</v>
+      </c>
+      <c r="AC17" s="20">
+        <v>0.154123292704263</v>
+      </c>
+      <c r="AD17" s="20">
+        <v>0.444</v>
+      </c>
+      <c r="AE17" s="20">
+        <v>0.760094627001101</v>
+      </c>
+      <c r="AF17" s="20">
+        <v>0.23760510078</v>
+      </c>
+      <c r="AG17" s="20">
+        <v>0.2070482</v>
+      </c>
+      <c r="AH17" s="22">
         <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="AI17" s="22" t="e">
+        <v>0.483024937566168</v>
+      </c>
+      <c r="AI17" s="22">
         <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="AJ17" s="22" t="e">
+        <v>0.73996392416256</v>
+      </c>
+      <c r="AJ17" s="22">
         <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="AK17" s="22" t="e">
+        <v>0.2152673583739</v>
+      </c>
+      <c r="AK17" s="22">
         <f t="shared" si="4"/>
-        <v>#DIV/0!</v>
+        <v>0.192467097915542</v>
       </c>
     </row>
     <row r="18" ht="19" customHeight="1" spans="1:37">
-      <c r="A18" s="23" t="s">
+      <c r="A18" s="7" t="s">
         <v>33</v>
       </c>
       <c r="B18" s="21"/>
@@ -2660,291 +2794,291 @@
       <c r="AF18" s="21"/>
       <c r="AG18" s="21"/>
       <c r="AH18" s="22" t="e">
-        <f t="shared" si="1"/>
+        <f>AVERAGE(AD18,Z18,V18,R18,N18,J18,F18)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="AI18" s="22" t="e">
-        <f t="shared" si="2"/>
+        <f>AVERAGE(AE18,AA18,W18,S18,O18,K18,G18)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="AJ18" s="22" t="e">
-        <f t="shared" si="3"/>
+        <f>AVERAGE(AF18,AB18,X18,T18,P18,L18,H18)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="AK18" s="22" t="e">
-        <f t="shared" si="4"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="19" spans="1:37">
-      <c r="A19" s="18" t="s">
+        <f>AVERAGE(AG18,AC18,Y18,U18,Q18,M18,I18)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="19" ht="19" customHeight="1" spans="1:37">
+      <c r="A19" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="B19" s="19"/>
-      <c r="C19" s="19"/>
-      <c r="D19" s="19"/>
-      <c r="E19" s="19"/>
-      <c r="F19" s="19"/>
-      <c r="G19" s="19"/>
-      <c r="H19" s="19"/>
-      <c r="I19" s="19"/>
-      <c r="J19" s="19"/>
-      <c r="K19" s="19"/>
-      <c r="L19" s="19"/>
-      <c r="M19" s="19"/>
-      <c r="N19" s="19"/>
-      <c r="O19" s="19"/>
-      <c r="P19" s="19"/>
-      <c r="Q19" s="19"/>
-      <c r="R19" s="19"/>
-      <c r="S19" s="19"/>
-      <c r="T19" s="19"/>
-      <c r="U19" s="19"/>
-      <c r="V19" s="19"/>
-      <c r="W19" s="19"/>
-      <c r="X19" s="19"/>
-      <c r="Y19" s="19"/>
-      <c r="Z19" s="19"/>
-      <c r="AA19" s="19"/>
-      <c r="AB19" s="19"/>
-      <c r="AC19" s="19"/>
-      <c r="AD19" s="19"/>
-      <c r="AE19" s="19"/>
-      <c r="AF19" s="19"/>
-      <c r="AG19" s="19"/>
-      <c r="AH19" s="19"/>
-      <c r="AI19" s="19"/>
-      <c r="AJ19" s="19"/>
-      <c r="AK19" s="19"/>
-    </row>
-    <row r="20" spans="1:37">
-      <c r="A20" s="7" t="s">
+      <c r="B19" s="21"/>
+      <c r="C19" s="21"/>
+      <c r="D19" s="21"/>
+      <c r="E19" s="21"/>
+      <c r="F19" s="21"/>
+      <c r="G19" s="21"/>
+      <c r="H19" s="21"/>
+      <c r="I19" s="21"/>
+      <c r="J19" s="21"/>
+      <c r="K19" s="21"/>
+      <c r="L19" s="21"/>
+      <c r="M19" s="21"/>
+      <c r="N19" s="21"/>
+      <c r="O19" s="21"/>
+      <c r="P19" s="21"/>
+      <c r="Q19" s="21"/>
+      <c r="R19" s="21"/>
+      <c r="S19" s="21"/>
+      <c r="T19" s="21"/>
+      <c r="U19" s="21"/>
+      <c r="V19" s="21"/>
+      <c r="W19" s="21"/>
+      <c r="X19" s="21"/>
+      <c r="Y19" s="21"/>
+      <c r="Z19" s="21"/>
+      <c r="AA19" s="21"/>
+      <c r="AB19" s="21"/>
+      <c r="AC19" s="21"/>
+      <c r="AD19" s="21"/>
+      <c r="AE19" s="21"/>
+      <c r="AF19" s="21"/>
+      <c r="AG19" s="21"/>
+      <c r="AH19" s="22" t="e">
+        <f>AVERAGE(AD19,Z19,V19,R19,N19,J19,F19)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AI19" s="22" t="e">
+        <f>AVERAGE(AE19,AA19,W19,S19,O19,K19,G19)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AJ19" s="22" t="e">
+        <f>AVERAGE(AF19,AB19,X19,T19,P19,L19,H19)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AK19" s="22" t="e">
+        <f>AVERAGE(AG19,AC19,Y19,U19,Q19,M19,I19)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="20" ht="19" customHeight="1" spans="1:37">
+      <c r="A20" s="23" t="s">
+        <v>35</v>
+      </c>
+      <c r="B20" s="21"/>
+      <c r="C20" s="21"/>
+      <c r="D20" s="21"/>
+      <c r="E20" s="21"/>
+      <c r="F20" s="21"/>
+      <c r="G20" s="21"/>
+      <c r="H20" s="21"/>
+      <c r="I20" s="21"/>
+      <c r="J20" s="21"/>
+      <c r="K20" s="21"/>
+      <c r="L20" s="21"/>
+      <c r="M20" s="21"/>
+      <c r="N20" s="21"/>
+      <c r="O20" s="21"/>
+      <c r="P20" s="21"/>
+      <c r="Q20" s="21"/>
+      <c r="R20" s="21"/>
+      <c r="S20" s="21"/>
+      <c r="T20" s="21"/>
+      <c r="U20" s="21"/>
+      <c r="V20" s="21"/>
+      <c r="W20" s="21"/>
+      <c r="X20" s="21"/>
+      <c r="Y20" s="21"/>
+      <c r="Z20" s="21"/>
+      <c r="AA20" s="21"/>
+      <c r="AB20" s="21"/>
+      <c r="AC20" s="21"/>
+      <c r="AD20" s="21"/>
+      <c r="AE20" s="21"/>
+      <c r="AF20" s="21"/>
+      <c r="AG20" s="21"/>
+      <c r="AH20" s="22" t="e">
+        <f>AVERAGE(AD20,Z20,V20,R20,N20,J20,F20)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AI20" s="22" t="e">
+        <f>AVERAGE(AE20,AA20,W20,S20,O20,K20,G20)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AJ20" s="22" t="e">
+        <f>AVERAGE(AF20,AB20,X20,T20,P20,L20,H20)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AK20" s="22" t="e">
+        <f>AVERAGE(AG20,AC20,Y20,U20,Q20,M20,I20)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="21" spans="1:37">
+      <c r="A21" s="18" t="s">
+        <v>36</v>
+      </c>
+      <c r="B21" s="19"/>
+      <c r="C21" s="19"/>
+      <c r="D21" s="19"/>
+      <c r="E21" s="19"/>
+      <c r="F21" s="19"/>
+      <c r="G21" s="19"/>
+      <c r="H21" s="19"/>
+      <c r="I21" s="19"/>
+      <c r="J21" s="19"/>
+      <c r="K21" s="19"/>
+      <c r="L21" s="19"/>
+      <c r="M21" s="19"/>
+      <c r="N21" s="19"/>
+      <c r="O21" s="19"/>
+      <c r="P21" s="19"/>
+      <c r="Q21" s="19"/>
+      <c r="R21" s="19"/>
+      <c r="S21" s="19"/>
+      <c r="T21" s="19"/>
+      <c r="U21" s="19"/>
+      <c r="V21" s="19"/>
+      <c r="W21" s="19"/>
+      <c r="X21" s="19"/>
+      <c r="Y21" s="19"/>
+      <c r="Z21" s="19"/>
+      <c r="AA21" s="19"/>
+      <c r="AB21" s="19"/>
+      <c r="AC21" s="19"/>
+      <c r="AD21" s="19"/>
+      <c r="AE21" s="19"/>
+      <c r="AF21" s="19"/>
+      <c r="AG21" s="19"/>
+      <c r="AH21" s="19"/>
+      <c r="AI21" s="19"/>
+      <c r="AJ21" s="19"/>
+      <c r="AK21" s="19"/>
+    </row>
+    <row r="22" spans="1:37">
+      <c r="A22" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="B20" s="21">
+      <c r="B22" s="21">
         <v>0.449</v>
       </c>
-      <c r="C20" s="21">
+      <c r="C22" s="21">
         <v>0.523530814595046</v>
       </c>
-      <c r="D20" s="21">
+      <c r="D22" s="21">
         <v>0.5431775</v>
       </c>
-      <c r="E20" s="21">
+      <c r="E22" s="21">
         <v>0.54615</v>
       </c>
-      <c r="F20" s="21">
+      <c r="F22" s="21">
         <v>0.118354137771613</v>
       </c>
-      <c r="G20" s="21">
+      <c r="G22" s="21">
         <v>0.608906434353696</v>
       </c>
-      <c r="H20" s="21">
+      <c r="H22" s="21">
         <v>0.707916088765603</v>
       </c>
-      <c r="I20" s="21">
+      <c r="I22" s="21">
         <v>0.767267683772538</v>
       </c>
-      <c r="J20" s="21">
+      <c r="J22" s="21">
         <v>0.5805</v>
       </c>
-      <c r="K20" s="21">
+      <c r="K22" s="21">
         <v>0.576300279546115</v>
       </c>
-      <c r="L20" s="21">
+      <c r="L22" s="21">
         <v>0.40117125</v>
       </c>
-      <c r="M20" s="21">
+      <c r="M22" s="21">
         <v>0.405724999999999</v>
       </c>
-      <c r="N20" s="21">
+      <c r="N22" s="21">
         <v>0.886977886977886</v>
       </c>
-      <c r="O20" s="21">
+      <c r="O22" s="21">
         <v>0.68519076103684</v>
       </c>
-      <c r="P20" s="21">
+      <c r="P22" s="21">
         <v>0.10002457002457</v>
       </c>
-      <c r="Q20" s="21">
+      <c r="Q22" s="21">
         <v>0.0753480753480753</v>
       </c>
-      <c r="R20" s="21">
+      <c r="R22" s="21">
         <v>0.475446428571428</v>
       </c>
-      <c r="S20" s="21">
+      <c r="S22" s="21">
         <v>0.531045849565478</v>
       </c>
-      <c r="T20" s="21">
+      <c r="T22" s="21">
         <v>0.481640625</v>
       </c>
-      <c r="U20" s="21">
+      <c r="U22" s="21">
         <v>0.481026785714285</v>
       </c>
-      <c r="V20" s="21">
+      <c r="V22" s="21">
         <v>0.6</v>
       </c>
-      <c r="W20" s="21">
+      <c r="W22" s="21">
         <v>0.505866666666666</v>
       </c>
-      <c r="X20" s="21">
+      <c r="X22" s="21">
         <v>0.39886</v>
       </c>
-      <c r="Y20" s="21">
+      <c r="Y22" s="21">
         <v>0.399</v>
       </c>
-      <c r="Z20" s="21">
+      <c r="Z22" s="21">
         <v>0.805155420773313</v>
       </c>
-      <c r="AA20" s="21">
+      <c r="AA22" s="21">
         <v>0.510249730704126</v>
       </c>
-      <c r="AB20" s="21">
+      <c r="AB22" s="21">
         <v>0.194412433661865</v>
       </c>
-      <c r="AC20" s="21">
+      <c r="AC22" s="21">
         <v>0.194465504169825</v>
       </c>
-      <c r="AD20" s="21">
+      <c r="AD22" s="21">
         <v>0.342</v>
       </c>
-      <c r="AE20" s="21">
+      <c r="AE22" s="21">
         <v>0.556764251053164</v>
       </c>
-      <c r="AF20" s="21">
+      <c r="AF22" s="21">
         <v>0.626095</v>
       </c>
-      <c r="AG20" s="21">
+      <c r="AG22" s="21">
         <v>0.6345</v>
       </c>
-      <c r="AH20" s="24">
-        <f t="shared" ref="AH20:AK20" si="5">AVERAGE(AD20,Z20,V20,R20,N20,J20,F20)</f>
+      <c r="AH22" s="24">
+        <f t="shared" ref="AH22:AK22" si="5">AVERAGE(AD22,Z22,V22,R22,N22,J22,F22)</f>
         <v>0.544061982013463</v>
       </c>
-      <c r="AI20" s="25">
+      <c r="AI22" s="25">
         <f t="shared" si="5"/>
         <v>0.567760567560869</v>
       </c>
-      <c r="AJ20" s="25">
+      <c r="AJ22" s="25">
         <f t="shared" si="5"/>
         <v>0.41573142392172</v>
       </c>
-      <c r="AK20" s="25">
+      <c r="AK22" s="25">
         <f t="shared" si="5"/>
         <v>0.422476149857817</v>
       </c>
     </row>
-    <row r="21" spans="1:37">
-      <c r="A21" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="B21" s="21"/>
-      <c r="C21" s="21"/>
-      <c r="D21" s="21"/>
-      <c r="E21" s="21"/>
-      <c r="F21" s="21"/>
-      <c r="G21" s="21"/>
-      <c r="H21" s="21"/>
-      <c r="I21" s="21"/>
-      <c r="J21" s="21"/>
-      <c r="K21" s="21"/>
-      <c r="L21" s="21"/>
-      <c r="M21" s="21"/>
-      <c r="N21" s="21"/>
-      <c r="O21" s="21"/>
-      <c r="P21" s="21"/>
-      <c r="Q21" s="21"/>
-      <c r="R21" s="21"/>
-      <c r="S21" s="21"/>
-      <c r="T21" s="21"/>
-      <c r="U21" s="21"/>
-      <c r="V21" s="21"/>
-      <c r="W21" s="21"/>
-      <c r="X21" s="21"/>
-      <c r="Y21" s="21"/>
-      <c r="Z21" s="21"/>
-      <c r="AA21" s="21"/>
-      <c r="AB21" s="21"/>
-      <c r="AC21" s="21"/>
-      <c r="AD21" s="21"/>
-      <c r="AE21" s="21"/>
-      <c r="AF21" s="21"/>
-      <c r="AG21" s="21"/>
-      <c r="AH21" s="24" t="e">
-        <f t="shared" ref="AH21:AH29" si="6">AVERAGE(AD21,Z21,V21,R21,N21,J21,F21)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="AI21" s="25" t="e">
-        <f t="shared" ref="AI21:AI29" si="7">AVERAGE(AE21,AA21,W21,S21,O21,K21,G21)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="AJ21" s="25" t="e">
-        <f t="shared" ref="AJ21:AJ29" si="8">AVERAGE(AF21,AB21,X21,T21,P21,L21,H21)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="AK21" s="25" t="e">
-        <f t="shared" ref="AK21:AK29" si="9">AVERAGE(AG21,AC21,Y21,U21,Q21,M21,I21)</f>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="22" spans="1:37">
-      <c r="A22" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="B22" s="26"/>
-      <c r="C22" s="21"/>
-      <c r="D22" s="21"/>
-      <c r="E22" s="21"/>
-      <c r="F22" s="21"/>
-      <c r="G22" s="21"/>
-      <c r="H22" s="21"/>
-      <c r="I22" s="21"/>
-      <c r="J22" s="21"/>
-      <c r="K22" s="21"/>
-      <c r="L22" s="21"/>
-      <c r="M22" s="21"/>
-      <c r="N22" s="21"/>
-      <c r="O22" s="21"/>
-      <c r="P22" s="21"/>
-      <c r="Q22" s="21"/>
-      <c r="R22" s="21"/>
-      <c r="S22" s="21"/>
-      <c r="T22" s="21"/>
-      <c r="U22" s="21"/>
-      <c r="V22" s="21"/>
-      <c r="W22" s="21"/>
-      <c r="X22" s="21"/>
-      <c r="Y22" s="21"/>
-      <c r="Z22" s="21"/>
-      <c r="AA22" s="21"/>
-      <c r="AB22" s="21"/>
-      <c r="AC22" s="21"/>
-      <c r="AD22" s="21"/>
-      <c r="AE22" s="21"/>
-      <c r="AF22" s="21"/>
-      <c r="AG22" s="21"/>
-      <c r="AH22" s="24" t="e">
-        <f t="shared" si="6"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="AI22" s="25" t="e">
-        <f t="shared" si="7"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="AJ22" s="25" t="e">
-        <f t="shared" si="8"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="AK22" s="25" t="e">
-        <f t="shared" si="9"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
     <row r="23" spans="1:37">
       <c r="A23" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="B23" s="26"/>
+        <v>22</v>
+      </c>
+      <c r="B23" s="21"/>
       <c r="C23" s="21"/>
       <c r="D23" s="21"/>
       <c r="E23" s="21"/>
@@ -2977,27 +3111,27 @@
       <c r="AF23" s="21"/>
       <c r="AG23" s="21"/>
       <c r="AH23" s="24" t="e">
-        <f t="shared" si="6"/>
+        <f t="shared" ref="AH23:AH31" si="6">AVERAGE(AD23,Z23,V23,R23,N23,J23,F23)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="AI23" s="25" t="e">
-        <f t="shared" si="7"/>
+        <f t="shared" ref="AI23:AI31" si="7">AVERAGE(AE23,AA23,W23,S23,O23,K23,G23)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="AJ23" s="25" t="e">
-        <f t="shared" si="8"/>
+        <f t="shared" ref="AJ23:AJ31" si="8">AVERAGE(AF23,AB23,X23,T23,P23,L23,H23)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="AK23" s="25" t="e">
-        <f t="shared" si="9"/>
+        <f t="shared" ref="AK23:AK31" si="9">AVERAGE(AG23,AC23,Y23,U23,Q23,M23,I23)</f>
         <v>#DIV/0!</v>
       </c>
     </row>
     <row r="24" spans="1:37">
       <c r="A24" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="B24" s="21"/>
+        <v>23</v>
+      </c>
+      <c r="B24" s="26"/>
       <c r="C24" s="21"/>
       <c r="D24" s="21"/>
       <c r="E24" s="21"/>
@@ -3048,9 +3182,9 @@
     </row>
     <row r="25" spans="1:37">
       <c r="A25" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="B25" s="21"/>
+        <v>24</v>
+      </c>
+      <c r="B25" s="26"/>
       <c r="C25" s="21"/>
       <c r="D25" s="21"/>
       <c r="E25" s="21"/>
@@ -3101,7 +3235,7 @@
     </row>
     <row r="26" spans="1:37">
       <c r="A26" s="7" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B26" s="21"/>
       <c r="C26" s="21"/>
@@ -3123,10 +3257,10 @@
       <c r="S26" s="21"/>
       <c r="T26" s="21"/>
       <c r="U26" s="21"/>
-      <c r="V26" s="27"/>
-      <c r="W26" s="27"/>
-      <c r="X26" s="27"/>
-      <c r="Y26" s="27"/>
+      <c r="V26" s="21"/>
+      <c r="W26" s="21"/>
+      <c r="X26" s="21"/>
+      <c r="Y26" s="21"/>
       <c r="Z26" s="21"/>
       <c r="AA26" s="21"/>
       <c r="AB26" s="21"/>
@@ -3152,9 +3286,9 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="27" ht="19" customHeight="1" spans="1:37">
+    <row r="27" spans="1:37">
       <c r="A27" s="7" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="B27" s="21"/>
       <c r="C27" s="21"/>
@@ -3176,10 +3310,10 @@
       <c r="S27" s="21"/>
       <c r="T27" s="21"/>
       <c r="U27" s="21"/>
-      <c r="V27" s="28"/>
-      <c r="W27" s="28"/>
-      <c r="X27" s="28"/>
-      <c r="Y27" s="28"/>
+      <c r="V27" s="21"/>
+      <c r="W27" s="21"/>
+      <c r="X27" s="21"/>
+      <c r="Y27" s="21"/>
       <c r="Z27" s="21"/>
       <c r="AA27" s="21"/>
       <c r="AB27" s="21"/>
@@ -3205,9 +3339,9 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="28" ht="19" customHeight="1" spans="1:37">
+    <row r="28" spans="1:37">
       <c r="A28" s="7" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="B28" s="21"/>
       <c r="C28" s="21"/>
@@ -3282,10 +3416,10 @@
       <c r="S29" s="21"/>
       <c r="T29" s="21"/>
       <c r="U29" s="21"/>
-      <c r="V29" s="27"/>
-      <c r="W29" s="27"/>
-      <c r="X29" s="27"/>
-      <c r="Y29" s="27"/>
+      <c r="V29" s="28"/>
+      <c r="W29" s="28"/>
+      <c r="X29" s="28"/>
+      <c r="Y29" s="28"/>
       <c r="Z29" s="21"/>
       <c r="AA29" s="21"/>
       <c r="AB29" s="21"/>
@@ -3311,549 +3445,553 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="34" customHeight="1" spans="1:37">
-      <c r="A34" s="29" t="s">
+    <row r="30" ht="19" customHeight="1" spans="1:37">
+      <c r="A30" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="B30" s="21"/>
+      <c r="C30" s="21"/>
+      <c r="D30" s="21"/>
+      <c r="E30" s="21"/>
+      <c r="F30" s="21"/>
+      <c r="G30" s="21"/>
+      <c r="H30" s="21"/>
+      <c r="I30" s="21"/>
+      <c r="J30" s="21"/>
+      <c r="K30" s="21"/>
+      <c r="L30" s="21"/>
+      <c r="M30" s="21"/>
+      <c r="N30" s="21"/>
+      <c r="O30" s="21"/>
+      <c r="P30" s="21"/>
+      <c r="Q30" s="21"/>
+      <c r="R30" s="21"/>
+      <c r="S30" s="21"/>
+      <c r="T30" s="21"/>
+      <c r="U30" s="21"/>
+      <c r="V30" s="27"/>
+      <c r="W30" s="27"/>
+      <c r="X30" s="27"/>
+      <c r="Y30" s="27"/>
+      <c r="Z30" s="21"/>
+      <c r="AA30" s="21"/>
+      <c r="AB30" s="21"/>
+      <c r="AC30" s="21"/>
+      <c r="AD30" s="21"/>
+      <c r="AE30" s="21"/>
+      <c r="AF30" s="21"/>
+      <c r="AG30" s="21"/>
+      <c r="AH30" s="24" t="e">
+        <f t="shared" si="6"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AI30" s="25" t="e">
+        <f t="shared" si="7"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AJ30" s="25" t="e">
+        <f t="shared" si="8"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AK30" s="25" t="e">
+        <f t="shared" si="9"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="31" ht="19" customHeight="1" spans="1:37">
+      <c r="A31" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="B31" s="21"/>
+      <c r="C31" s="21"/>
+      <c r="D31" s="21"/>
+      <c r="E31" s="21"/>
+      <c r="F31" s="21"/>
+      <c r="G31" s="21"/>
+      <c r="H31" s="21"/>
+      <c r="I31" s="21"/>
+      <c r="J31" s="21"/>
+      <c r="K31" s="21"/>
+      <c r="L31" s="21"/>
+      <c r="M31" s="21"/>
+      <c r="N31" s="21"/>
+      <c r="O31" s="21"/>
+      <c r="P31" s="21"/>
+      <c r="Q31" s="21"/>
+      <c r="R31" s="21"/>
+      <c r="S31" s="21"/>
+      <c r="T31" s="21"/>
+      <c r="U31" s="21"/>
+      <c r="V31" s="27"/>
+      <c r="W31" s="27"/>
+      <c r="X31" s="27"/>
+      <c r="Y31" s="27"/>
+      <c r="Z31" s="21"/>
+      <c r="AA31" s="21"/>
+      <c r="AB31" s="21"/>
+      <c r="AC31" s="21"/>
+      <c r="AD31" s="21"/>
+      <c r="AE31" s="21"/>
+      <c r="AF31" s="21"/>
+      <c r="AG31" s="21"/>
+      <c r="AH31" s="24" t="e">
+        <f t="shared" si="6"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AI31" s="25" t="e">
+        <f t="shared" si="7"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AJ31" s="25" t="e">
+        <f t="shared" si="8"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AK31" s="25" t="e">
+        <f t="shared" si="9"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="36" customHeight="1" spans="1:37">
+      <c r="A36" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="B34" s="30" t="s">
-        <v>35</v>
-      </c>
-      <c r="C34" s="2"/>
-      <c r="D34" s="2"/>
-      <c r="E34" s="2"/>
-      <c r="F34" s="2"/>
-      <c r="G34" s="2"/>
-      <c r="H34" s="2"/>
-      <c r="I34" s="2"/>
-      <c r="J34" s="2"/>
-      <c r="K34" s="2"/>
-      <c r="L34" s="2"/>
-      <c r="M34" s="2"/>
-      <c r="N34" s="2"/>
-      <c r="O34" s="2"/>
-      <c r="P34" s="2"/>
-      <c r="Q34" s="2"/>
-      <c r="R34" s="2"/>
-      <c r="S34" s="2"/>
-      <c r="T34" s="2"/>
-      <c r="U34" s="2"/>
-      <c r="V34" s="2"/>
-      <c r="W34" s="2"/>
-      <c r="X34" s="2"/>
-      <c r="Y34" s="2"/>
-      <c r="Z34" s="2"/>
-      <c r="AA34" s="2"/>
-      <c r="AB34" s="2"/>
-      <c r="AC34" s="2"/>
-      <c r="AD34" s="2"/>
-      <c r="AE34" s="2"/>
-      <c r="AF34" s="2"/>
-      <c r="AG34" s="2"/>
-      <c r="AH34" s="2"/>
-      <c r="AI34" s="2"/>
-      <c r="AJ34" s="2"/>
-      <c r="AK34" s="2"/>
-    </row>
-    <row r="35" spans="1:37">
-      <c r="A35" s="30"/>
-      <c r="B35" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="C35" s="5"/>
-      <c r="D35" s="5"/>
-      <c r="E35" s="6"/>
-      <c r="F35" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="G35" s="7"/>
-      <c r="H35" s="7"/>
-      <c r="I35" s="7"/>
-      <c r="J35" s="7"/>
-      <c r="K35" s="7"/>
-      <c r="L35" s="7"/>
-      <c r="M35" s="7"/>
-      <c r="N35" s="7"/>
-      <c r="O35" s="7"/>
-      <c r="P35" s="7"/>
-      <c r="Q35" s="7"/>
-      <c r="R35" s="7"/>
-      <c r="S35" s="7"/>
-      <c r="T35" s="7"/>
-      <c r="U35" s="7"/>
-      <c r="V35" s="7"/>
-      <c r="W35" s="7"/>
-      <c r="X35" s="7"/>
-      <c r="Y35" s="7"/>
-      <c r="Z35" s="7"/>
-      <c r="AA35" s="7"/>
-      <c r="AB35" s="7"/>
-      <c r="AC35" s="7"/>
-      <c r="AD35" s="7"/>
-      <c r="AE35" s="7"/>
-      <c r="AF35" s="7"/>
-      <c r="AG35" s="7"/>
-      <c r="AH35" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="AI35" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="AJ35" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="AK35" s="8" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="36" spans="1:37">
-      <c r="A36" s="30"/>
-      <c r="B36" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="C36" s="9"/>
-      <c r="D36" s="9"/>
-      <c r="E36" s="9"/>
-      <c r="F36" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="G36" s="10"/>
-      <c r="H36" s="10"/>
-      <c r="I36" s="10"/>
-      <c r="J36" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="K36" s="10"/>
-      <c r="L36" s="10"/>
-      <c r="M36" s="10"/>
-      <c r="N36" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="O36" s="10"/>
-      <c r="P36" s="10"/>
-      <c r="Q36" s="10"/>
-      <c r="R36" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="S36" s="10"/>
-      <c r="T36" s="10"/>
-      <c r="U36" s="10"/>
-      <c r="V36" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="W36" s="10"/>
-      <c r="X36" s="10"/>
-      <c r="Y36" s="10"/>
-      <c r="Z36" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="AA36" s="10"/>
-      <c r="AB36" s="10"/>
-      <c r="AC36" s="10"/>
-      <c r="AD36" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="AE36" s="10"/>
-      <c r="AF36" s="10"/>
-      <c r="AG36" s="10"/>
-      <c r="AH36" s="8"/>
-      <c r="AI36" s="8"/>
-      <c r="AJ36" s="8"/>
-      <c r="AK36" s="8"/>
+      <c r="B36" s="30" t="s">
+        <v>37</v>
+      </c>
+      <c r="C36" s="2"/>
+      <c r="D36" s="2"/>
+      <c r="E36" s="2"/>
+      <c r="F36" s="2"/>
+      <c r="G36" s="2"/>
+      <c r="H36" s="2"/>
+      <c r="I36" s="2"/>
+      <c r="J36" s="2"/>
+      <c r="K36" s="2"/>
+      <c r="L36" s="2"/>
+      <c r="M36" s="2"/>
+      <c r="N36" s="2"/>
+      <c r="O36" s="2"/>
+      <c r="P36" s="2"/>
+      <c r="Q36" s="2"/>
+      <c r="R36" s="2"/>
+      <c r="S36" s="2"/>
+      <c r="T36" s="2"/>
+      <c r="U36" s="2"/>
+      <c r="V36" s="2"/>
+      <c r="W36" s="2"/>
+      <c r="X36" s="2"/>
+      <c r="Y36" s="2"/>
+      <c r="Z36" s="2"/>
+      <c r="AA36" s="2"/>
+      <c r="AB36" s="2"/>
+      <c r="AC36" s="2"/>
+      <c r="AD36" s="2"/>
+      <c r="AE36" s="2"/>
+      <c r="AF36" s="2"/>
+      <c r="AG36" s="2"/>
+      <c r="AH36" s="2"/>
+      <c r="AI36" s="2"/>
+      <c r="AJ36" s="2"/>
+      <c r="AK36" s="2"/>
     </row>
     <row r="37" spans="1:37">
       <c r="A37" s="30"/>
-      <c r="B37" s="13" t="s">
+      <c r="B37" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="C37" s="5"/>
+      <c r="D37" s="5"/>
+      <c r="E37" s="6"/>
+      <c r="F37" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="G37" s="7"/>
+      <c r="H37" s="7"/>
+      <c r="I37" s="7"/>
+      <c r="J37" s="7"/>
+      <c r="K37" s="7"/>
+      <c r="L37" s="7"/>
+      <c r="M37" s="7"/>
+      <c r="N37" s="7"/>
+      <c r="O37" s="7"/>
+      <c r="P37" s="7"/>
+      <c r="Q37" s="7"/>
+      <c r="R37" s="7"/>
+      <c r="S37" s="7"/>
+      <c r="T37" s="7"/>
+      <c r="U37" s="7"/>
+      <c r="V37" s="7"/>
+      <c r="W37" s="7"/>
+      <c r="X37" s="7"/>
+      <c r="Y37" s="7"/>
+      <c r="Z37" s="7"/>
+      <c r="AA37" s="7"/>
+      <c r="AB37" s="7"/>
+      <c r="AC37" s="7"/>
+      <c r="AD37" s="7"/>
+      <c r="AE37" s="7"/>
+      <c r="AF37" s="7"/>
+      <c r="AG37" s="7"/>
+      <c r="AH37" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="AI37" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="AJ37" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="AK37" s="8" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="38" spans="1:37">
+      <c r="A38" s="30"/>
+      <c r="B38" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="C38" s="9"/>
+      <c r="D38" s="9"/>
+      <c r="E38" s="9"/>
+      <c r="F38" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="G38" s="10"/>
+      <c r="H38" s="10"/>
+      <c r="I38" s="10"/>
+      <c r="J38" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="K38" s="10"/>
+      <c r="L38" s="10"/>
+      <c r="M38" s="10"/>
+      <c r="N38" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="O38" s="10"/>
+      <c r="P38" s="10"/>
+      <c r="Q38" s="10"/>
+      <c r="R38" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="S38" s="10"/>
+      <c r="T38" s="10"/>
+      <c r="U38" s="10"/>
+      <c r="V38" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="W38" s="10"/>
+      <c r="X38" s="10"/>
+      <c r="Y38" s="10"/>
+      <c r="Z38" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="AA38" s="10"/>
+      <c r="AB38" s="10"/>
+      <c r="AC38" s="10"/>
+      <c r="AD38" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="AE38" s="10"/>
+      <c r="AF38" s="10"/>
+      <c r="AG38" s="10"/>
+      <c r="AH38" s="8"/>
+      <c r="AI38" s="8"/>
+      <c r="AJ38" s="8"/>
+      <c r="AK38" s="8"/>
+    </row>
+    <row r="39" spans="1:37">
+      <c r="A39" s="30"/>
+      <c r="B39" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="C37" s="14" t="s">
+      <c r="C39" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="D37" s="14" t="s">
+      <c r="D39" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="E37" s="15" t="s">
+      <c r="E39" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="F37" s="9" t="s">
+      <c r="F39" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="G37" s="16" t="s">
+      <c r="G39" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="H37" s="16" t="s">
+      <c r="H39" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="I37" s="17" t="s">
+      <c r="I39" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="J37" s="13" t="s">
+      <c r="J39" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="K37" s="14" t="s">
+      <c r="K39" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="L37" s="14" t="s">
+      <c r="L39" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="M37" s="15" t="s">
+      <c r="M39" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="N37" s="13" t="s">
+      <c r="N39" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="O37" s="14" t="s">
+      <c r="O39" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="P37" s="14" t="s">
+      <c r="P39" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="Q37" s="15" t="s">
+      <c r="Q39" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="R37" s="13" t="s">
+      <c r="R39" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="S37" s="14" t="s">
+      <c r="S39" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="T37" s="14" t="s">
+      <c r="T39" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="U37" s="15" t="s">
+      <c r="U39" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="V37" s="13" t="s">
+      <c r="V39" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="W37" s="14" t="s">
+      <c r="W39" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="X37" s="14" t="s">
+      <c r="X39" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="Y37" s="15" t="s">
+      <c r="Y39" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="Z37" s="13" t="s">
+      <c r="Z39" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="AA37" s="14" t="s">
+      <c r="AA39" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="AB37" s="14" t="s">
+      <c r="AB39" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="AC37" s="15" t="s">
+      <c r="AC39" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="AD37" s="13" t="s">
+      <c r="AD39" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="AE37" s="14" t="s">
+      <c r="AE39" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="AF37" s="14" t="s">
+      <c r="AF39" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="AG37" s="15" t="s">
+      <c r="AG39" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="AH37" s="8"/>
-      <c r="AI37" s="8"/>
-      <c r="AJ37" s="8"/>
-      <c r="AK37" s="8"/>
-    </row>
-    <row r="38" spans="1:37">
-      <c r="A38" s="18" t="s">
+      <c r="AH39" s="8"/>
+      <c r="AI39" s="8"/>
+      <c r="AJ39" s="8"/>
+      <c r="AK39" s="8"/>
+    </row>
+    <row r="40" spans="1:37">
+      <c r="A40" s="18" t="s">
         <v>20</v>
       </c>
-      <c r="B38" s="19"/>
-      <c r="C38" s="19"/>
-      <c r="D38" s="19"/>
-      <c r="E38" s="19"/>
-      <c r="F38" s="19"/>
-      <c r="G38" s="19"/>
-      <c r="H38" s="19"/>
-      <c r="I38" s="19"/>
-      <c r="J38" s="19"/>
-      <c r="K38" s="19"/>
-      <c r="L38" s="19"/>
-      <c r="M38" s="19"/>
-      <c r="N38" s="19"/>
-      <c r="O38" s="19"/>
-      <c r="P38" s="19"/>
-      <c r="Q38" s="19"/>
-      <c r="R38" s="19"/>
-      <c r="S38" s="19"/>
-      <c r="T38" s="19"/>
-      <c r="U38" s="19"/>
-      <c r="V38" s="19"/>
-      <c r="W38" s="19"/>
-      <c r="X38" s="19"/>
-      <c r="Y38" s="19"/>
-      <c r="Z38" s="19"/>
-      <c r="AA38" s="19"/>
-      <c r="AB38" s="19"/>
-      <c r="AC38" s="19"/>
-      <c r="AD38" s="19"/>
-      <c r="AE38" s="19"/>
-      <c r="AF38" s="19"/>
-      <c r="AG38" s="19"/>
-      <c r="AH38" s="19"/>
-      <c r="AI38" s="19"/>
-      <c r="AJ38" s="19"/>
-      <c r="AK38" s="19"/>
-    </row>
-    <row r="39" spans="1:37">
-      <c r="A39" s="5" t="s">
+      <c r="B40" s="19"/>
+      <c r="C40" s="19"/>
+      <c r="D40" s="19"/>
+      <c r="E40" s="19"/>
+      <c r="F40" s="19"/>
+      <c r="G40" s="19"/>
+      <c r="H40" s="19"/>
+      <c r="I40" s="19"/>
+      <c r="J40" s="19"/>
+      <c r="K40" s="19"/>
+      <c r="L40" s="19"/>
+      <c r="M40" s="19"/>
+      <c r="N40" s="19"/>
+      <c r="O40" s="19"/>
+      <c r="P40" s="19"/>
+      <c r="Q40" s="19"/>
+      <c r="R40" s="19"/>
+      <c r="S40" s="19"/>
+      <c r="T40" s="19"/>
+      <c r="U40" s="19"/>
+      <c r="V40" s="19"/>
+      <c r="W40" s="19"/>
+      <c r="X40" s="19"/>
+      <c r="Y40" s="19"/>
+      <c r="Z40" s="19"/>
+      <c r="AA40" s="19"/>
+      <c r="AB40" s="19"/>
+      <c r="AC40" s="19"/>
+      <c r="AD40" s="19"/>
+      <c r="AE40" s="19"/>
+      <c r="AF40" s="19"/>
+      <c r="AG40" s="19"/>
+      <c r="AH40" s="19"/>
+      <c r="AI40" s="19"/>
+      <c r="AJ40" s="19"/>
+      <c r="AK40" s="19"/>
+    </row>
+    <row r="41" spans="1:37">
+      <c r="A41" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="B39" s="20">
+      <c r="B41" s="20">
         <v>0.522</v>
       </c>
-      <c r="C39" s="20">
+      <c r="C41" s="20">
         <v>0.563751422754452</v>
       </c>
-      <c r="D39" s="20">
+      <c r="D41" s="20">
         <v>0.464219</v>
       </c>
-      <c r="E39" s="20">
+      <c r="E41" s="20">
         <v>0.4676</v>
       </c>
-      <c r="F39" s="21">
+      <c r="F41" s="21">
         <f>F6</f>
         <v>0.0929264909847434</v>
       </c>
-      <c r="G39" s="21">
-        <f t="shared" ref="G39:U39" si="10">G6</f>
+      <c r="G41" s="21">
+        <f t="shared" ref="G41:U41" si="10">G6</f>
         <v>0.591062906669506</v>
       </c>
-      <c r="H39" s="21">
+      <c r="H41" s="21">
         <f t="shared" si="10"/>
         <v>0.705082917244567</v>
       </c>
-      <c r="I39" s="21">
+      <c r="I41" s="21">
         <f t="shared" si="10"/>
         <v>0.726558021266759</v>
       </c>
-      <c r="J39" s="21">
+      <c r="J41" s="21">
         <f t="shared" si="10"/>
         <v>0.482</v>
       </c>
-      <c r="K39" s="21">
+      <c r="K41" s="21">
         <f t="shared" si="10"/>
         <v>0.581368954164597</v>
       </c>
-      <c r="L39" s="21">
+      <c r="L41" s="21">
         <f t="shared" si="10"/>
         <v>0.46800755</v>
       </c>
-      <c r="M39" s="21">
+      <c r="M41" s="21">
         <f t="shared" si="10"/>
         <v>0.473095</v>
       </c>
-      <c r="N39" s="21">
+      <c r="N41" s="21">
         <f t="shared" si="10"/>
         <v>0.86076986076986</v>
       </c>
-      <c r="O39" s="21">
+      <c r="O41" s="21">
         <f t="shared" si="10"/>
         <v>0.619443667095763</v>
       </c>
-      <c r="P39" s="21">
+      <c r="P41" s="21">
         <f t="shared" si="10"/>
         <v>0.127618755118755</v>
       </c>
-      <c r="Q39" s="21">
+      <c r="Q41" s="21">
         <f t="shared" si="10"/>
         <v>0.115929565929565</v>
       </c>
-      <c r="R39" s="21">
+      <c r="R41" s="21">
         <f t="shared" si="10"/>
         <v>0.446428571428571</v>
       </c>
-      <c r="S39" s="21">
+      <c r="S41" s="21">
         <f t="shared" si="10"/>
         <v>0.496441532258064</v>
       </c>
-      <c r="T39" s="21">
+      <c r="T41" s="21">
         <f t="shared" si="10"/>
         <v>0.515220957589285</v>
       </c>
-      <c r="U39" s="21">
+      <c r="U41" s="21">
         <f t="shared" si="10"/>
         <v>0.515216517857142</v>
       </c>
-      <c r="V39" s="21">
+      <c r="V41" s="21">
         <f>B6</f>
         <v>0.459</v>
       </c>
-      <c r="W39" s="21">
+      <c r="W41" s="21">
         <f>C6</f>
         <v>0.559838353086151</v>
       </c>
-      <c r="X39" s="21">
+      <c r="X41" s="21">
         <f>D6</f>
         <v>0.5002526</v>
       </c>
-      <c r="Y39" s="21">
+      <c r="Y41" s="21">
         <f>E6</f>
         <v>0.50314</v>
       </c>
-      <c r="Z39" s="21">
+      <c r="Z41" s="21">
         <f>Z6</f>
         <v>0.733889310083396</v>
       </c>
-      <c r="AA39" s="21">
+      <c r="AA41" s="21">
         <f>AA6</f>
         <v>0.53642043982953</v>
       </c>
-      <c r="AB39" s="21">
+      <c r="AB41" s="21">
         <f>AB6</f>
         <v>0.260898407884761</v>
       </c>
-      <c r="AC39" s="21">
+      <c r="AC41" s="21">
         <f>AC6</f>
         <v>0.26163760424564</v>
       </c>
-      <c r="AD39" s="26">
+      <c r="AD41" s="26">
         <f>V6</f>
         <v>0.516</v>
       </c>
-      <c r="AE39" s="26">
+      <c r="AE41" s="26">
         <f>W6</f>
         <v>0.546303414696649</v>
       </c>
-      <c r="AF39" s="26">
+      <c r="AF41" s="26">
         <f>X6</f>
         <v>0.472356200708616</v>
       </c>
-      <c r="AG39" s="26">
+      <c r="AG41" s="26">
         <f>Y6</f>
         <v>0.474764523809523</v>
       </c>
-      <c r="AH39" s="22">
-        <f>AVERAGE(B39,Z39,V39,R39,N39,J39,F39)</f>
+      <c r="AH41" s="22">
+        <f>AVERAGE(B41,Z41,V41,R41,N41,J41,F41)</f>
         <v>0.513859176180939</v>
       </c>
-      <c r="AI39" s="22">
-        <f t="shared" ref="AI39:AK39" si="11">AVERAGE(C39,AA39,W39,S39,O39,K39,G39)</f>
+      <c r="AI41" s="22">
+        <f t="shared" ref="AI41:AK41" si="11">AVERAGE(C41,AA41,W41,S41,O41,K41,G41)</f>
         <v>0.564046753694009</v>
       </c>
-      <c r="AJ39" s="22">
+      <c r="AJ41" s="22">
         <f t="shared" si="11"/>
         <v>0.434471455405338</v>
       </c>
-      <c r="AK39" s="22">
+      <c r="AK41" s="22">
         <f t="shared" si="11"/>
         <v>0.437596672757015</v>
       </c>
     </row>
-    <row r="40" spans="1:37">
-      <c r="A40" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="F40" s="21"/>
-      <c r="G40" s="21"/>
-      <c r="H40" s="21"/>
-      <c r="I40" s="21"/>
-      <c r="J40" s="21"/>
-      <c r="K40" s="21"/>
-      <c r="L40" s="21"/>
-      <c r="M40" s="21"/>
-      <c r="N40" s="21"/>
-      <c r="O40" s="21"/>
-      <c r="P40" s="21"/>
-      <c r="Q40" s="21"/>
-      <c r="R40" s="21"/>
-      <c r="S40" s="21"/>
-      <c r="T40" s="21"/>
-      <c r="U40" s="21"/>
-      <c r="V40" s="21"/>
-      <c r="W40" s="21"/>
-      <c r="X40" s="21"/>
-      <c r="Y40" s="21"/>
-      <c r="Z40" s="21"/>
-      <c r="AA40" s="21"/>
-      <c r="AB40" s="21"/>
-      <c r="AC40" s="21"/>
-      <c r="AD40" s="20"/>
-      <c r="AE40" s="20"/>
-      <c r="AF40" s="20"/>
-      <c r="AG40" s="20"/>
-      <c r="AH40" s="22" t="e">
-        <f>AVERAGE(AD40,Z40,V40,R40,N40,J40,F40)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="AI40" s="22" t="e">
-        <f>AVERAGE(AE40,AA40,W40,S40,O40,K40,G40)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="AJ40" s="22" t="e">
-        <f>AVERAGE(AF40,AB40,X40,T40,P40,L40,H40)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="AK40" s="22" t="e">
-        <f>AVERAGE(AG40,AC40,Y40,U40,Q40,M40,I40)</f>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="41" spans="1:37">
-      <c r="A41" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="B41" s="26"/>
-      <c r="C41" s="21"/>
-      <c r="D41" s="21"/>
-      <c r="E41" s="21"/>
-      <c r="F41" s="21"/>
-      <c r="G41" s="21"/>
-      <c r="H41" s="21"/>
-      <c r="I41" s="21"/>
-      <c r="J41" s="21"/>
-      <c r="K41" s="21"/>
-      <c r="L41" s="21"/>
-      <c r="M41" s="21"/>
-      <c r="N41" s="21"/>
-      <c r="O41" s="21"/>
-      <c r="P41" s="21"/>
-      <c r="Q41" s="21"/>
-      <c r="R41" s="21"/>
-      <c r="S41" s="21"/>
-      <c r="T41" s="21"/>
-      <c r="U41" s="21"/>
-      <c r="V41" s="21"/>
-      <c r="W41" s="21"/>
-      <c r="X41" s="21"/>
-      <c r="Y41" s="21"/>
-      <c r="Z41" s="21"/>
-      <c r="AA41" s="21"/>
-      <c r="AB41" s="21"/>
-      <c r="AC41" s="21"/>
-      <c r="AD41" s="20"/>
-      <c r="AE41" s="20"/>
-      <c r="AF41" s="20"/>
-      <c r="AG41" s="20"/>
-      <c r="AH41" s="22" t="e">
-        <f>AVERAGE(AD41,Z41,V41,R41,N41,J41,F41)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="AI41" s="22" t="e">
-        <f>AVERAGE(AE41,AA41,W41,S41,O41,K41,G41)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="AJ41" s="22" t="e">
-        <f>AVERAGE(AF41,AB41,X41,T41,P41,L41,H41)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="AK41" s="22" t="e">
-        <f>AVERAGE(AG41,AC41,Y41,U41,Q41,M41,I41)</f>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
     <row r="42" spans="1:37">
       <c r="A42" s="5" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="F42" s="21"/>
       <c r="G42" s="21"/>
@@ -3901,9 +4039,13 @@
       </c>
     </row>
     <row r="43" spans="1:37">
-      <c r="A43" s="6" t="s">
-        <v>25</v>
-      </c>
+      <c r="A43" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="B43" s="26"/>
+      <c r="C43" s="21"/>
+      <c r="D43" s="21"/>
+      <c r="E43" s="21"/>
       <c r="F43" s="21"/>
       <c r="G43" s="21"/>
       <c r="H43" s="21"/>
@@ -3950,8 +4092,8 @@
       </c>
     </row>
     <row r="44" spans="1:37">
-      <c r="A44" s="6" t="s">
-        <v>26</v>
+      <c r="A44" s="5" t="s">
+        <v>24</v>
       </c>
       <c r="F44" s="21"/>
       <c r="G44" s="21"/>
@@ -3973,10 +4115,10 @@
       <c r="W44" s="21"/>
       <c r="X44" s="21"/>
       <c r="Y44" s="21"/>
-      <c r="Z44" s="20"/>
-      <c r="AA44" s="20"/>
-      <c r="AB44" s="20"/>
-      <c r="AC44" s="20"/>
+      <c r="Z44" s="21"/>
+      <c r="AA44" s="21"/>
+      <c r="AB44" s="21"/>
+      <c r="AC44" s="21"/>
       <c r="AD44" s="20"/>
       <c r="AE44" s="20"/>
       <c r="AF44" s="20"/>
@@ -4000,587 +4142,711 @@
     </row>
     <row r="45" spans="1:37">
       <c r="A45" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="F45" s="21"/>
+      <c r="G45" s="21"/>
+      <c r="H45" s="21"/>
+      <c r="I45" s="21"/>
+      <c r="J45" s="21"/>
+      <c r="K45" s="21"/>
+      <c r="L45" s="21"/>
+      <c r="M45" s="21"/>
+      <c r="N45" s="21"/>
+      <c r="O45" s="21"/>
+      <c r="P45" s="21"/>
+      <c r="Q45" s="21"/>
+      <c r="R45" s="21"/>
+      <c r="S45" s="21"/>
+      <c r="T45" s="21"/>
+      <c r="U45" s="21"/>
+      <c r="V45" s="21"/>
+      <c r="W45" s="21"/>
+      <c r="X45" s="21"/>
+      <c r="Y45" s="21"/>
+      <c r="Z45" s="21"/>
+      <c r="AA45" s="21"/>
+      <c r="AB45" s="21"/>
+      <c r="AC45" s="21"/>
+      <c r="AD45" s="20"/>
+      <c r="AE45" s="20"/>
+      <c r="AF45" s="20"/>
+      <c r="AG45" s="20"/>
+      <c r="AH45" s="22" t="e">
+        <f>AVERAGE(AD45,Z45,V45,R45,N45,J45,F45)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AI45" s="22" t="e">
+        <f>AVERAGE(AE45,AA45,W45,S45,O45,K45,G45)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AJ45" s="22" t="e">
+        <f>AVERAGE(AF45,AB45,X45,T45,P45,L45,H45)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AK45" s="22" t="e">
+        <f>AVERAGE(AG45,AC45,Y45,U45,Q45,M45,I45)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="46" spans="1:37">
+      <c r="A46" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="B46" s="20">
+        <v>0.63</v>
+      </c>
+      <c r="C46" s="20">
+        <v>0.779165594165594</v>
+      </c>
+      <c r="D46" s="20">
+        <v>0.1804025</v>
+      </c>
+      <c r="E46" s="20">
+        <v>0.120049999999999</v>
+      </c>
+      <c r="F46" s="20">
+        <v>0.0931576514100785</v>
+      </c>
+      <c r="G46" s="20">
+        <v>0.601355561051481</v>
+      </c>
+      <c r="H46" s="20">
+        <v>0.259225543226999</v>
+      </c>
+      <c r="I46" s="20">
+        <v>0.359715672676837</v>
+      </c>
+      <c r="J46" s="20">
+        <v>0.5075</v>
+      </c>
+      <c r="K46" s="20">
+        <v>0.658902753119451</v>
+      </c>
+      <c r="L46" s="20">
+        <v>0.232607499999999</v>
+      </c>
+      <c r="M46" s="20">
+        <v>0.09764</v>
+      </c>
+      <c r="N46" s="20">
+        <v>0.854217854217854</v>
+      </c>
+      <c r="O46" s="20">
+        <v>0.705171986598726</v>
+      </c>
+      <c r="P46" s="20">
+        <v>0.165569205569205</v>
+      </c>
+      <c r="Q46" s="20">
+        <v>0.226699426699426</v>
+      </c>
+      <c r="R46" s="20">
+        <v>0.392857142857142</v>
+      </c>
+      <c r="S46" s="20">
+        <v>0.555637951203208</v>
+      </c>
+      <c r="T46" s="20">
+        <v>0.321577008928571</v>
+      </c>
+      <c r="U46" s="20">
+        <v>0.283861607142857</v>
+      </c>
+      <c r="V46" s="20">
+        <v>0.491</v>
+      </c>
+      <c r="W46" s="20">
+        <v>0.633649302373969</v>
+      </c>
+      <c r="X46" s="20">
+        <v>0.238406799999999</v>
+      </c>
+      <c r="Y46" s="20">
+        <v>0.04312</v>
+      </c>
+      <c r="Z46" s="20">
+        <v>0.862774829416224</v>
+      </c>
+      <c r="AA46" s="20">
+        <v>0.598180388196797</v>
+      </c>
+      <c r="AB46" s="20">
+        <v>0.13882486732373</v>
+      </c>
+      <c r="AC46" s="20">
+        <v>0.185367702805155</v>
+      </c>
+      <c r="AD46" s="20">
+        <v>0.522</v>
+      </c>
+      <c r="AE46" s="20">
+        <v>0.767004921528078</v>
+      </c>
+      <c r="AF46" s="20">
+        <v>0.196102449999999</v>
+      </c>
+      <c r="AG46" s="20">
+        <v>0.0943699999999998</v>
+      </c>
+      <c r="AH46" s="22">
+        <f>AVERAGE(AD46,Z46,V46,R46,N46,J46,F46)</f>
+        <v>0.531929639700185</v>
+      </c>
+      <c r="AI46" s="22">
+        <f>AVERAGE(AE46,AA46,W46,S46,O46,K46,G46)</f>
+        <v>0.645700409153101</v>
+      </c>
+      <c r="AJ46" s="22">
+        <f>AVERAGE(AF46,AB46,X46,T46,P46,L46,H46)</f>
+        <v>0.221759053578357</v>
+      </c>
+      <c r="AK46" s="22">
+        <f>AVERAGE(AG46,AC46,Y46,U46,Q46,M46,I46)</f>
+        <v>0.184396344189182</v>
+      </c>
+    </row>
+    <row r="47" spans="1:37">
+      <c r="A47" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="B45" s="20">
+      <c r="B47" s="20">
         <v>0.599</v>
       </c>
-      <c r="C45" s="20">
+      <c r="C47" s="20">
         <v>0.817343119663279</v>
       </c>
-      <c r="D45" s="20">
+      <c r="D47" s="20">
         <v>0.185360578775778</v>
       </c>
-      <c r="E45" s="20">
+      <c r="E47" s="20">
         <v>0.155985665665666</v>
       </c>
-      <c r="F45" s="20">
+      <c r="F47" s="20">
         <v>0.079750346740638</v>
       </c>
-      <c r="G45" s="20">
+      <c r="G47" s="20">
         <v>0.673908674901434</v>
       </c>
-      <c r="H45" s="20">
+      <c r="H47" s="20">
         <v>0.170577145476961</v>
       </c>
-      <c r="I45" s="20">
+      <c r="I47" s="20">
         <v>0.177568192094313</v>
       </c>
-      <c r="J45" s="20">
+      <c r="J47" s="20">
         <v>0.49</v>
       </c>
-      <c r="K45" s="20">
+      <c r="K47" s="20">
         <v>0.774051120448179</v>
       </c>
-      <c r="L45" s="20">
+      <c r="L47" s="20">
         <v>0.226415243444445</v>
       </c>
-      <c r="M45" s="20">
+      <c r="M47" s="20">
         <v>0.174536665166666</v>
       </c>
-      <c r="N45" s="20">
+      <c r="N47" s="20">
         <v>0.864045864045864</v>
       </c>
-      <c r="O45" s="20">
+      <c r="O47" s="20">
         <v>0.739833266716153</v>
       </c>
-      <c r="P45" s="20">
+      <c r="P47" s="20">
         <v>0.225538201838202</v>
       </c>
-      <c r="Q45" s="20">
+      <c r="Q47" s="20">
         <v>0.285582854763854</v>
       </c>
-      <c r="R45" s="20">
+      <c r="R47" s="20">
         <v>0.392857142857142</v>
       </c>
-      <c r="S45" s="20">
+      <c r="S47" s="20">
         <v>0.555637951203208</v>
       </c>
-      <c r="T45" s="20">
+      <c r="T47" s="20">
         <v>0.321577008928571</v>
       </c>
-      <c r="U45" s="20">
+      <c r="U47" s="20">
         <v>0.283861607142857</v>
       </c>
-      <c r="V45" s="20">
+      <c r="V47" s="20">
         <v>0.448</v>
       </c>
-      <c r="W45" s="20">
+      <c r="W47" s="20">
         <v>0.675759009446169</v>
       </c>
-      <c r="X45" s="20">
+      <c r="X47" s="20">
         <v>0.294500122222222</v>
       </c>
-      <c r="Y45" s="20">
+      <c r="Y47" s="20">
         <v>0.25001</v>
       </c>
-      <c r="Z45" s="20">
+      <c r="Z47" s="20">
         <v>0.846095526914329</v>
       </c>
-      <c r="AA45" s="20">
+      <c r="AA47" s="20">
         <v>0.773840422338753</v>
       </c>
-      <c r="AB45" s="20">
+      <c r="AB47" s="20">
         <v>0.105001297279083</v>
       </c>
-      <c r="AC45" s="20">
+      <c r="AC47" s="20">
         <v>0.0981602223907</v>
       </c>
-      <c r="AD45" s="20">
+      <c r="AD47" s="20">
         <v>0.514</v>
       </c>
-      <c r="AE45" s="20">
+      <c r="AE47" s="20">
         <v>0.795903988727162</v>
       </c>
-      <c r="AF45" s="20">
+      <c r="AF47" s="20">
         <v>0.213415091506172</v>
       </c>
-      <c r="AG45" s="20">
+      <c r="AG47" s="20">
         <v>0.198892444444444</v>
-      </c>
-      <c r="AH45" s="22">
-        <f>AVERAGE(B45,Z45,V45,R45,N45,J45,F45)</f>
-        <v>0.531392697222568</v>
-      </c>
-      <c r="AI45" s="22">
-        <f>AVERAGE(C45,AA45,W45,S45,O45,K45,G45)</f>
-        <v>0.715767652102454</v>
-      </c>
-      <c r="AJ45" s="22">
-        <f>AVERAGE(D45,AB45,X45,T45,P45,L45,H45)</f>
-        <v>0.218424228280752</v>
-      </c>
-      <c r="AK45" s="22">
-        <f>AVERAGE(E45,AC45,Y45,U45,Q45,M45,I45)</f>
-        <v>0.203672172460579</v>
-      </c>
-    </row>
-    <row r="46" spans="1:37">
-      <c r="A46" s="31" t="s">
-        <v>28</v>
-      </c>
-      <c r="B46" s="20"/>
-      <c r="C46" s="20"/>
-      <c r="D46" s="20"/>
-      <c r="E46" s="20"/>
-      <c r="F46" s="20"/>
-      <c r="G46" s="20"/>
-      <c r="H46" s="20"/>
-      <c r="I46" s="20"/>
-      <c r="J46" s="20"/>
-      <c r="K46" s="20"/>
-      <c r="L46" s="20"/>
-      <c r="M46" s="20"/>
-      <c r="N46" s="20"/>
-      <c r="O46" s="20"/>
-      <c r="P46" s="20"/>
-      <c r="Q46" s="20"/>
-      <c r="R46" s="20"/>
-      <c r="S46" s="20"/>
-      <c r="T46" s="20"/>
-      <c r="U46" s="20"/>
-      <c r="V46" s="20"/>
-      <c r="W46" s="20"/>
-      <c r="X46" s="20"/>
-      <c r="Y46" s="20"/>
-      <c r="Z46" s="20"/>
-      <c r="AA46" s="20"/>
-      <c r="AB46" s="20"/>
-      <c r="AC46" s="20"/>
-      <c r="AD46" s="20"/>
-      <c r="AE46" s="20"/>
-      <c r="AF46" s="20"/>
-      <c r="AG46" s="20"/>
-      <c r="AH46" s="22" t="e">
-        <f>AVERAGE(B46,Z46,V46,R46,N46,J46,F46)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="AI46" s="22" t="e">
-        <f>AVERAGE(C46,AA46,W46,S46,O46,K46,G46)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="AJ46" s="22" t="e">
-        <f>AVERAGE(D46,AB46,X46,T46,P46,L46,H46)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="AK46" s="22" t="e">
-        <f>AVERAGE(E46,AC46,Y46,U46,Q46,M46,I46)</f>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="47" spans="1:37">
-      <c r="A47" s="31" t="s">
-        <v>29</v>
-      </c>
-      <c r="B47" s="20">
-        <v>0.615</v>
-      </c>
-      <c r="C47" s="20">
-        <v>0.781828740365325</v>
-      </c>
-      <c r="D47" s="20">
-        <v>0.21092440533</v>
-      </c>
-      <c r="E47" s="20">
-        <v>0.203806699999999</v>
-      </c>
-      <c r="F47" s="20">
-        <v>0.09500693481276</v>
-      </c>
-      <c r="G47" s="20">
-        <v>0.572767103877096</v>
-      </c>
-      <c r="H47" s="20">
-        <v>0.184885994105409</v>
-      </c>
-      <c r="I47" s="20">
-        <v>0.200303791030975</v>
-      </c>
-      <c r="J47" s="20">
-        <v>0.4955</v>
-      </c>
-      <c r="K47" s="20">
-        <v>0.721920975599023</v>
-      </c>
-      <c r="L47" s="20">
-        <v>0.272423652885</v>
-      </c>
-      <c r="M47" s="20">
-        <v>0.23755615</v>
-      </c>
-      <c r="N47" s="20">
-        <v>0.77067977067977</v>
-      </c>
-      <c r="O47" s="20">
-        <v>0.586479049643236</v>
-      </c>
-      <c r="P47" s="20">
-        <v>0.454282147927927</v>
-      </c>
-      <c r="Q47" s="20">
-        <v>0.479011302211302</v>
-      </c>
-      <c r="R47" s="20">
-        <v>0.345982142857142</v>
-      </c>
-      <c r="S47" s="20">
-        <v>0.515644610811406</v>
-      </c>
-      <c r="T47" s="20">
-        <v>0.321333928683035</v>
-      </c>
-      <c r="U47" s="20">
-        <v>0.304998883928571</v>
-      </c>
-      <c r="V47" s="20">
-        <v>0.464</v>
-      </c>
-      <c r="W47" s="20">
-        <v>0.649685972079258</v>
-      </c>
-      <c r="X47" s="20">
-        <v>0.33994890441</v>
-      </c>
-      <c r="Y47" s="20">
-        <v>0.3196059</v>
-      </c>
-      <c r="Z47" s="20">
-        <v>0.857467778620166</v>
-      </c>
-      <c r="AA47" s="20">
-        <v>0.725426566585774</v>
-      </c>
-      <c r="AB47" s="20">
-        <v>0.101252548544351</v>
-      </c>
-      <c r="AC47" s="20">
-        <v>0.0959777862016678</v>
-      </c>
-      <c r="AD47" s="20">
-        <v>0.476</v>
-      </c>
-      <c r="AE47" s="20">
-        <v>0.784230867919687</v>
-      </c>
-      <c r="AF47" s="20">
-        <v>0.23900901144</v>
-      </c>
-      <c r="AG47" s="20">
-        <v>0.2311128</v>
       </c>
       <c r="AH47" s="22">
         <f>AVERAGE(B47,Z47,V47,R47,N47,J47,F47)</f>
-        <v>0.520519518138548</v>
+        <v>0.531392697222568</v>
       </c>
       <c r="AI47" s="22">
         <f>AVERAGE(C47,AA47,W47,S47,O47,K47,G47)</f>
-        <v>0.650536145565874</v>
+        <v>0.715767652102454</v>
       </c>
       <c r="AJ47" s="22">
         <f>AVERAGE(D47,AB47,X47,T47,P47,L47,H47)</f>
-        <v>0.269293083126532</v>
+        <v>0.218424228280752</v>
       </c>
       <c r="AK47" s="22">
         <f>AVERAGE(E47,AC47,Y47,U47,Q47,M47,I47)</f>
+        <v>0.203672172460579</v>
+      </c>
+    </row>
+    <row r="48" spans="1:37">
+      <c r="A48" s="31" t="s">
+        <v>28</v>
+      </c>
+      <c r="B48" s="20">
+        <v>0.603</v>
+      </c>
+      <c r="C48" s="20">
+        <v>0.802924921989548</v>
+      </c>
+      <c r="D48" s="20">
+        <v>0.191650355666666</v>
+      </c>
+      <c r="E48" s="20">
+        <v>0.188307</v>
+      </c>
+      <c r="F48" s="20">
+        <v>0.073509015256588</v>
+      </c>
+      <c r="G48" s="20">
+        <v>0.548507936956276</v>
+      </c>
+      <c r="H48" s="20">
+        <v>0.141347717953685</v>
+      </c>
+      <c r="I48" s="20">
+        <v>0.147970488379132</v>
+      </c>
+      <c r="J48" s="20">
+        <v>0.472</v>
+      </c>
+      <c r="K48" s="20">
+        <v>0.721796553993323</v>
+      </c>
+      <c r="L48" s="20">
+        <v>0.27422350243865</v>
+      </c>
+      <c r="M48" s="20">
+        <v>0.25964515019839</v>
+      </c>
+      <c r="N48" s="20">
+        <v>0.865683865683865</v>
+      </c>
+      <c r="O48" s="20">
+        <v>0.713250224980963</v>
+      </c>
+      <c r="P48" s="20">
+        <v>0.411531322517534</v>
+      </c>
+      <c r="Q48" s="20">
+        <v>0.42334698356577</v>
+      </c>
+      <c r="R48" s="20">
+        <v>0.381696428571428</v>
+      </c>
+      <c r="S48" s="20">
+        <v>0.524837967361243</v>
+      </c>
+      <c r="T48" s="20">
+        <v>0.365038779761904</v>
+      </c>
+      <c r="U48" s="20">
+        <v>0.363035714285714</v>
+      </c>
+      <c r="V48" s="20">
+        <v>0.423</v>
+      </c>
+      <c r="W48" s="20">
+        <v>0.584409864342752</v>
+      </c>
+      <c r="X48" s="20">
+        <v>0.355160194</v>
+      </c>
+      <c r="Y48" s="20">
+        <v>0.346805999999999</v>
+      </c>
+      <c r="Z48" s="20">
+        <v>0.851402577710386</v>
+      </c>
+      <c r="AA48" s="20">
+        <v>0.674784651171243</v>
+      </c>
+      <c r="AB48" s="20">
+        <v>0.109995849970516</v>
+      </c>
+      <c r="AC48" s="20">
+        <v>0.109707606772807</v>
+      </c>
+      <c r="AD48" s="20">
+        <v>0.504</v>
+      </c>
+      <c r="AE48" s="20">
+        <v>0.815420186891961</v>
+      </c>
+      <c r="AF48" s="20">
+        <v>0.2051379947263</v>
+      </c>
+      <c r="AG48" s="20">
+        <v>0.205485638961038</v>
+      </c>
+      <c r="AH48" s="22">
+        <f>AVERAGE(B48,Z48,V48,R48,N48,J48,F48)</f>
+        <v>0.524327412460324</v>
+      </c>
+      <c r="AI48" s="22">
+        <f>AVERAGE(C48,AA48,W48,S48,O48,K48,G48)</f>
+        <v>0.652930302970764</v>
+      </c>
+      <c r="AJ48" s="22">
+        <f>AVERAGE(D48,AB48,X48,T48,P48,L48,H48)</f>
+        <v>0.264135388901279</v>
+      </c>
+      <c r="AK48" s="22">
+        <f>AVERAGE(E48,AC48,Y48,U48,Q48,M48,I48)</f>
+        <v>0.262688420457402</v>
+      </c>
+    </row>
+    <row r="49" spans="1:37">
+      <c r="A49" s="31" t="s">
+        <v>29</v>
+      </c>
+      <c r="B49" s="20">
+        <v>0.615</v>
+      </c>
+      <c r="C49" s="20">
+        <v>0.781828740365325</v>
+      </c>
+      <c r="D49" s="20">
+        <v>0.21092440533</v>
+      </c>
+      <c r="E49" s="20">
+        <v>0.203806699999999</v>
+      </c>
+      <c r="F49" s="20">
+        <v>0.09500693481276</v>
+      </c>
+      <c r="G49" s="20">
+        <v>0.572767103877096</v>
+      </c>
+      <c r="H49" s="20">
+        <v>0.184885994105409</v>
+      </c>
+      <c r="I49" s="20">
+        <v>0.200303791030975</v>
+      </c>
+      <c r="J49" s="20">
+        <v>0.4955</v>
+      </c>
+      <c r="K49" s="20">
+        <v>0.721920975599023</v>
+      </c>
+      <c r="L49" s="20">
+        <v>0.272423652885</v>
+      </c>
+      <c r="M49" s="20">
+        <v>0.23755615</v>
+      </c>
+      <c r="N49" s="20">
+        <v>0.77067977067977</v>
+      </c>
+      <c r="O49" s="20">
+        <v>0.586479049643236</v>
+      </c>
+      <c r="P49" s="20">
+        <v>0.454282147927927</v>
+      </c>
+      <c r="Q49" s="20">
+        <v>0.479011302211302</v>
+      </c>
+      <c r="R49" s="20">
+        <v>0.345982142857142</v>
+      </c>
+      <c r="S49" s="20">
+        <v>0.515644610811406</v>
+      </c>
+      <c r="T49" s="20">
+        <v>0.321333928683035</v>
+      </c>
+      <c r="U49" s="20">
+        <v>0.304998883928571</v>
+      </c>
+      <c r="V49" s="20">
+        <v>0.464</v>
+      </c>
+      <c r="W49" s="20">
+        <v>0.649685972079258</v>
+      </c>
+      <c r="X49" s="20">
+        <v>0.33994890441</v>
+      </c>
+      <c r="Y49" s="20">
+        <v>0.3196059</v>
+      </c>
+      <c r="Z49" s="20">
+        <v>0.857467778620166</v>
+      </c>
+      <c r="AA49" s="20">
+        <v>0.725426566585774</v>
+      </c>
+      <c r="AB49" s="20">
+        <v>0.101252548544351</v>
+      </c>
+      <c r="AC49" s="20">
+        <v>0.0959777862016678</v>
+      </c>
+      <c r="AD49" s="20">
+        <v>0.476</v>
+      </c>
+      <c r="AE49" s="20">
+        <v>0.784230867919687</v>
+      </c>
+      <c r="AF49" s="20">
+        <v>0.23900901144</v>
+      </c>
+      <c r="AG49" s="20">
+        <v>0.2311128</v>
+      </c>
+      <c r="AH49" s="22">
+        <f>AVERAGE(B49,Z49,V49,R49,N49,J49,F49)</f>
+        <v>0.520519518138548</v>
+      </c>
+      <c r="AI49" s="22">
+        <f>AVERAGE(C49,AA49,W49,S49,O49,K49,G49)</f>
+        <v>0.650536145565874</v>
+      </c>
+      <c r="AJ49" s="22">
+        <f>AVERAGE(D49,AB49,X49,T49,P49,L49,H49)</f>
+        <v>0.269293083126532</v>
+      </c>
+      <c r="AK49" s="22">
+        <f>AVERAGE(E49,AC49,Y49,U49,Q49,M49,I49)</f>
         <v>0.263037216196074</v>
       </c>
     </row>
-    <row r="48" spans="1:37">
-      <c r="A48" s="18" t="s">
-        <v>34</v>
-      </c>
-      <c r="B48" s="19"/>
-      <c r="C48" s="19"/>
-      <c r="D48" s="19"/>
-      <c r="E48" s="19"/>
-      <c r="F48" s="19"/>
-      <c r="G48" s="19"/>
-      <c r="H48" s="19"/>
-      <c r="I48" s="19"/>
-      <c r="J48" s="19"/>
-      <c r="K48" s="19"/>
-      <c r="L48" s="19"/>
-      <c r="M48" s="19"/>
-      <c r="N48" s="19"/>
-      <c r="O48" s="19"/>
-      <c r="P48" s="19"/>
-      <c r="Q48" s="19"/>
-      <c r="R48" s="19"/>
-      <c r="S48" s="19"/>
-      <c r="T48" s="19"/>
-      <c r="U48" s="19"/>
-      <c r="V48" s="19"/>
-      <c r="W48" s="19"/>
-      <c r="X48" s="19"/>
-      <c r="Y48" s="19"/>
-      <c r="Z48" s="19"/>
-      <c r="AA48" s="19"/>
-      <c r="AB48" s="19"/>
-      <c r="AC48" s="19"/>
-      <c r="AD48" s="19"/>
-      <c r="AE48" s="19"/>
-      <c r="AF48" s="19"/>
-      <c r="AG48" s="19"/>
-      <c r="AH48" s="19"/>
-      <c r="AI48" s="19"/>
-      <c r="AJ48" s="19"/>
-      <c r="AK48" s="19"/>
-    </row>
-    <row r="49" spans="1:37">
-      <c r="A49" s="5" t="s">
+    <row r="50" spans="1:37">
+      <c r="A50" s="18" t="s">
+        <v>36</v>
+      </c>
+      <c r="B50" s="19"/>
+      <c r="C50" s="19"/>
+      <c r="D50" s="19"/>
+      <c r="E50" s="19"/>
+      <c r="F50" s="19"/>
+      <c r="G50" s="19"/>
+      <c r="H50" s="19"/>
+      <c r="I50" s="19"/>
+      <c r="J50" s="19"/>
+      <c r="K50" s="19"/>
+      <c r="L50" s="19"/>
+      <c r="M50" s="19"/>
+      <c r="N50" s="19"/>
+      <c r="O50" s="19"/>
+      <c r="P50" s="19"/>
+      <c r="Q50" s="19"/>
+      <c r="R50" s="19"/>
+      <c r="S50" s="19"/>
+      <c r="T50" s="19"/>
+      <c r="U50" s="19"/>
+      <c r="V50" s="19"/>
+      <c r="W50" s="19"/>
+      <c r="X50" s="19"/>
+      <c r="Y50" s="19"/>
+      <c r="Z50" s="19"/>
+      <c r="AA50" s="19"/>
+      <c r="AB50" s="19"/>
+      <c r="AC50" s="19"/>
+      <c r="AD50" s="19"/>
+      <c r="AE50" s="19"/>
+      <c r="AF50" s="19"/>
+      <c r="AG50" s="19"/>
+      <c r="AH50" s="19"/>
+      <c r="AI50" s="19"/>
+      <c r="AJ50" s="19"/>
+      <c r="AK50" s="19"/>
+    </row>
+    <row r="51" spans="1:37">
+      <c r="A51" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="B49" s="20">
+      <c r="B51" s="20">
         <v>0.614</v>
       </c>
-      <c r="C49" s="20">
+      <c r="C51" s="20">
         <v>0.552387301480143</v>
       </c>
-      <c r="D49" s="20">
+      <c r="D51" s="20">
         <v>0.378925399999999</v>
       </c>
-      <c r="E49" s="20">
+      <c r="E51" s="20">
         <v>0.38118</v>
       </c>
-      <c r="F49" s="21">
-        <f t="shared" ref="F49:I49" si="12">F20</f>
+      <c r="F51" s="21">
+        <f t="shared" ref="F51:I51" si="12">F22</f>
         <v>0.118354137771613</v>
       </c>
-      <c r="G49" s="21">
+      <c r="G51" s="21">
         <f t="shared" si="12"/>
         <v>0.608906434353696</v>
       </c>
-      <c r="H49" s="21">
+      <c r="H51" s="21">
         <f t="shared" si="12"/>
         <v>0.707916088765603</v>
       </c>
-      <c r="I49" s="21">
+      <c r="I51" s="21">
         <f t="shared" si="12"/>
         <v>0.767267683772538</v>
       </c>
-      <c r="J49" s="21">
-        <f t="shared" ref="J49:U49" si="13">J20</f>
+      <c r="J51" s="21">
+        <f t="shared" ref="J51:U51" si="13">J22</f>
         <v>0.5805</v>
       </c>
-      <c r="K49" s="21">
+      <c r="K51" s="21">
         <f t="shared" si="13"/>
         <v>0.576300279546115</v>
       </c>
-      <c r="L49" s="21">
+      <c r="L51" s="21">
         <f t="shared" si="13"/>
         <v>0.40117125</v>
       </c>
-      <c r="M49" s="21">
+      <c r="M51" s="21">
         <f t="shared" si="13"/>
         <v>0.405724999999999</v>
       </c>
-      <c r="N49" s="21">
+      <c r="N51" s="21">
         <f t="shared" si="13"/>
         <v>0.886977886977886</v>
       </c>
-      <c r="O49" s="21">
+      <c r="O51" s="21">
         <f t="shared" si="13"/>
         <v>0.68519076103684</v>
       </c>
-      <c r="P49" s="21">
+      <c r="P51" s="21">
         <f t="shared" si="13"/>
         <v>0.10002457002457</v>
       </c>
-      <c r="Q49" s="21">
+      <c r="Q51" s="21">
         <f t="shared" si="13"/>
         <v>0.0753480753480753</v>
       </c>
-      <c r="R49" s="21">
+      <c r="R51" s="21">
         <f t="shared" si="13"/>
         <v>0.475446428571428</v>
       </c>
-      <c r="S49" s="21">
+      <c r="S51" s="21">
         <f t="shared" si="13"/>
         <v>0.531045849565478</v>
       </c>
-      <c r="T49" s="21">
+      <c r="T51" s="21">
         <f t="shared" si="13"/>
         <v>0.481640625</v>
       </c>
-      <c r="U49" s="21">
+      <c r="U51" s="21">
         <f t="shared" si="13"/>
         <v>0.481026785714285</v>
       </c>
-      <c r="V49" s="21">
-        <f>B20</f>
+      <c r="V51" s="21">
+        <f>B22</f>
         <v>0.449</v>
       </c>
-      <c r="W49" s="21">
-        <f>C20</f>
+      <c r="W51" s="21">
+        <f>C22</f>
         <v>0.523530814595046</v>
       </c>
-      <c r="X49" s="21">
-        <f>D20</f>
+      <c r="X51" s="21">
+        <f>D22</f>
         <v>0.5431775</v>
       </c>
-      <c r="Y49" s="21">
-        <f>E20</f>
+      <c r="Y51" s="21">
+        <f>E22</f>
         <v>0.54615</v>
       </c>
-      <c r="Z49" s="21">
-        <f>Z20</f>
+      <c r="Z51" s="21">
+        <f>Z22</f>
         <v>0.805155420773313</v>
       </c>
-      <c r="AA49" s="21">
-        <f>AA20</f>
+      <c r="AA51" s="21">
+        <f>AA22</f>
         <v>0.510249730704126</v>
       </c>
-      <c r="AB49" s="21">
-        <f>AB20</f>
+      <c r="AB51" s="21">
+        <f>AB22</f>
         <v>0.194412433661865</v>
       </c>
-      <c r="AC49" s="21">
-        <f>AC20</f>
+      <c r="AC51" s="21">
+        <f>AC22</f>
         <v>0.194465504169825</v>
       </c>
-      <c r="AD49" s="26">
-        <f>V20</f>
+      <c r="AD51" s="26">
+        <f>V22</f>
         <v>0.6</v>
       </c>
-      <c r="AE49" s="26">
-        <f>W20</f>
+      <c r="AE51" s="26">
+        <f>W22</f>
         <v>0.505866666666666</v>
       </c>
-      <c r="AF49" s="26">
-        <f>X20</f>
+      <c r="AF51" s="26">
+        <f>X22</f>
         <v>0.39886</v>
       </c>
-      <c r="AG49" s="26">
-        <f>Y20</f>
+      <c r="AG51" s="26">
+        <f>Y22</f>
         <v>0.399</v>
       </c>
-      <c r="AH49" s="25">
-        <f t="shared" ref="AH49:AK49" si="14">AVERAGE(B49,Z49,V49,R49,N49,J49,F49)</f>
+      <c r="AH51" s="25">
+        <f t="shared" ref="AH51:AK51" si="14">AVERAGE(B51,Z51,V51,R51,N51,J51,F51)</f>
         <v>0.561347696299177</v>
       </c>
-      <c r="AI49" s="25">
+      <c r="AI51" s="25">
         <f t="shared" si="14"/>
         <v>0.569658738754492</v>
       </c>
-      <c r="AJ49" s="25">
+      <c r="AJ51" s="25">
         <f t="shared" si="14"/>
         <v>0.401038266778862</v>
       </c>
-      <c r="AK49" s="25">
+      <c r="AK51" s="25">
         <f t="shared" si="14"/>
         <v>0.407309007000675</v>
       </c>
     </row>
-    <row r="50" spans="1:37">
-      <c r="A50" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="F50" s="21"/>
-      <c r="G50" s="21"/>
-      <c r="H50" s="21"/>
-      <c r="I50" s="21"/>
-      <c r="J50" s="21"/>
-      <c r="K50" s="21"/>
-      <c r="L50" s="21"/>
-      <c r="M50" s="21"/>
-      <c r="N50" s="21"/>
-      <c r="O50" s="21"/>
-      <c r="P50" s="21"/>
-      <c r="Q50" s="21"/>
-      <c r="R50" s="21"/>
-      <c r="S50" s="21"/>
-      <c r="T50" s="21"/>
-      <c r="U50" s="21"/>
-      <c r="V50" s="21"/>
-      <c r="W50" s="21"/>
-      <c r="X50" s="21"/>
-      <c r="Y50" s="21"/>
-      <c r="Z50" s="21"/>
-      <c r="AA50" s="21"/>
-      <c r="AB50" s="21"/>
-      <c r="AC50" s="21"/>
-      <c r="AD50" s="21"/>
-      <c r="AE50" s="21"/>
-      <c r="AF50" s="21"/>
-      <c r="AG50" s="21"/>
-      <c r="AH50" s="25" t="e">
-        <f t="shared" ref="AH50:AH55" si="15">AVERAGE(AD50,Z50,V50,R50,N50,J50,F50)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="AI50" s="25" t="e">
-        <f t="shared" ref="AI50:AI55" si="16">AVERAGE(AE50,AA50,W50,S50,O50,K50,G50)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="AJ50" s="25" t="e">
-        <f t="shared" ref="AJ50:AJ55" si="17">AVERAGE(AF50,AB50,X50,T50,P50,L50,H50)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="AK50" s="25" t="e">
-        <f t="shared" ref="AK50:AK55" si="18">AVERAGE(AG50,AC50,Y50,U50,Q50,M50,I50)</f>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="51" spans="1:37">
-      <c r="A51" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="B51" s="26"/>
-      <c r="C51" s="21"/>
-      <c r="D51" s="21"/>
-      <c r="E51" s="21"/>
-      <c r="F51" s="21"/>
-      <c r="G51" s="21"/>
-      <c r="H51" s="21"/>
-      <c r="I51" s="21"/>
-      <c r="J51" s="21"/>
-      <c r="K51" s="21"/>
-      <c r="L51" s="21"/>
-      <c r="M51" s="21"/>
-      <c r="N51" s="21"/>
-      <c r="O51" s="21"/>
-      <c r="P51" s="21"/>
-      <c r="Q51" s="21"/>
-      <c r="R51" s="21"/>
-      <c r="S51" s="21"/>
-      <c r="T51" s="21"/>
-      <c r="U51" s="21"/>
-      <c r="V51" s="21"/>
-      <c r="W51" s="21"/>
-      <c r="X51" s="21"/>
-      <c r="Y51" s="21"/>
-      <c r="Z51" s="21"/>
-      <c r="AA51" s="21"/>
-      <c r="AB51" s="21"/>
-      <c r="AC51" s="21"/>
-      <c r="AD51" s="21"/>
-      <c r="AE51" s="21"/>
-      <c r="AF51" s="21"/>
-      <c r="AG51" s="21"/>
-      <c r="AH51" s="25" t="e">
-        <f t="shared" si="15"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="AI51" s="25" t="e">
-        <f t="shared" si="16"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="AJ51" s="25" t="e">
-        <f t="shared" si="17"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="AK51" s="25" t="e">
-        <f t="shared" si="18"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
     <row r="52" spans="1:37">
       <c r="A52" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="B52" s="26"/>
-      <c r="C52" s="21"/>
-      <c r="D52" s="21"/>
-      <c r="E52" s="21"/>
+        <v>22</v>
+      </c>
       <c r="F52" s="21"/>
       <c r="G52" s="21"/>
       <c r="H52" s="21"/>
@@ -4610,27 +4876,27 @@
       <c r="AF52" s="21"/>
       <c r="AG52" s="21"/>
       <c r="AH52" s="25" t="e">
-        <f t="shared" si="15"/>
+        <f t="shared" ref="AH52:AH57" si="15">AVERAGE(AD52,Z52,V52,R52,N52,J52,F52)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="AI52" s="25" t="e">
-        <f t="shared" si="16"/>
+        <f t="shared" ref="AI52:AI57" si="16">AVERAGE(AE52,AA52,W52,S52,O52,K52,G52)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="AJ52" s="25" t="e">
-        <f t="shared" si="17"/>
+        <f t="shared" ref="AJ52:AJ57" si="17">AVERAGE(AF52,AB52,X52,T52,P52,L52,H52)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="AK52" s="25" t="e">
-        <f t="shared" si="18"/>
+        <f t="shared" ref="AK52:AK57" si="18">AVERAGE(AG52,AC52,Y52,U52,Q52,M52,I52)</f>
         <v>#DIV/0!</v>
       </c>
     </row>
     <row r="53" spans="1:37">
-      <c r="A53" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="B53" s="21"/>
+      <c r="A53" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="B53" s="26"/>
       <c r="C53" s="21"/>
       <c r="D53" s="21"/>
       <c r="E53" s="21"/>
@@ -4680,10 +4946,10 @@
       </c>
     </row>
     <row r="54" spans="1:37">
-      <c r="A54" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="B54" s="21"/>
+      <c r="A54" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B54" s="26"/>
       <c r="C54" s="21"/>
       <c r="D54" s="21"/>
       <c r="E54" s="21"/>
@@ -4733,8 +4999,8 @@
       </c>
     </row>
     <row r="55" spans="1:37">
-      <c r="A55" s="31" t="s">
-        <v>28</v>
+      <c r="A55" s="6" t="s">
+        <v>25</v>
       </c>
       <c r="B55" s="21"/>
       <c r="C55" s="21"/>
@@ -4756,10 +5022,10 @@
       <c r="S55" s="21"/>
       <c r="T55" s="21"/>
       <c r="U55" s="21"/>
-      <c r="V55" s="20"/>
-      <c r="W55" s="20"/>
-      <c r="X55" s="20"/>
-      <c r="Y55" s="20"/>
+      <c r="V55" s="21"/>
+      <c r="W55" s="21"/>
+      <c r="X55" s="21"/>
+      <c r="Y55" s="21"/>
       <c r="Z55" s="21"/>
       <c r="AA55" s="21"/>
       <c r="AB55" s="21"/>
@@ -4786,8 +5052,114 @@
       </c>
     </row>
     <row r="56" spans="1:37">
-      <c r="A56" s="1" t="s">
-        <v>37</v>
+      <c r="A56" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="B56" s="21"/>
+      <c r="C56" s="21"/>
+      <c r="D56" s="21"/>
+      <c r="E56" s="21"/>
+      <c r="F56" s="21"/>
+      <c r="G56" s="21"/>
+      <c r="H56" s="21"/>
+      <c r="I56" s="21"/>
+      <c r="J56" s="21"/>
+      <c r="K56" s="21"/>
+      <c r="L56" s="21"/>
+      <c r="M56" s="21"/>
+      <c r="N56" s="21"/>
+      <c r="O56" s="21"/>
+      <c r="P56" s="21"/>
+      <c r="Q56" s="21"/>
+      <c r="R56" s="21"/>
+      <c r="S56" s="21"/>
+      <c r="T56" s="21"/>
+      <c r="U56" s="21"/>
+      <c r="V56" s="21"/>
+      <c r="W56" s="21"/>
+      <c r="X56" s="21"/>
+      <c r="Y56" s="21"/>
+      <c r="Z56" s="21"/>
+      <c r="AA56" s="21"/>
+      <c r="AB56" s="21"/>
+      <c r="AC56" s="21"/>
+      <c r="AD56" s="21"/>
+      <c r="AE56" s="21"/>
+      <c r="AF56" s="21"/>
+      <c r="AG56" s="21"/>
+      <c r="AH56" s="25" t="e">
+        <f t="shared" si="15"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AI56" s="25" t="e">
+        <f t="shared" si="16"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AJ56" s="25" t="e">
+        <f t="shared" si="17"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AK56" s="25" t="e">
+        <f t="shared" si="18"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="57" spans="1:37">
+      <c r="A57" s="31" t="s">
+        <v>28</v>
+      </c>
+      <c r="B57" s="21"/>
+      <c r="C57" s="21"/>
+      <c r="D57" s="21"/>
+      <c r="E57" s="21"/>
+      <c r="F57" s="21"/>
+      <c r="G57" s="21"/>
+      <c r="H57" s="21"/>
+      <c r="I57" s="21"/>
+      <c r="J57" s="21"/>
+      <c r="K57" s="21"/>
+      <c r="L57" s="21"/>
+      <c r="M57" s="21"/>
+      <c r="N57" s="21"/>
+      <c r="O57" s="21"/>
+      <c r="P57" s="21"/>
+      <c r="Q57" s="21"/>
+      <c r="R57" s="21"/>
+      <c r="S57" s="21"/>
+      <c r="T57" s="21"/>
+      <c r="U57" s="21"/>
+      <c r="V57" s="20"/>
+      <c r="W57" s="20"/>
+      <c r="X57" s="20"/>
+      <c r="Y57" s="20"/>
+      <c r="Z57" s="21"/>
+      <c r="AA57" s="21"/>
+      <c r="AB57" s="21"/>
+      <c r="AC57" s="21"/>
+      <c r="AD57" s="21"/>
+      <c r="AE57" s="21"/>
+      <c r="AF57" s="21"/>
+      <c r="AG57" s="21"/>
+      <c r="AH57" s="25" t="e">
+        <f t="shared" si="15"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AI57" s="25" t="e">
+        <f t="shared" si="16"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AJ57" s="25" t="e">
+        <f t="shared" si="17"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AK57" s="25" t="e">
+        <f t="shared" si="18"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="58" spans="1:37">
+      <c r="A58" s="1" t="s">
+        <v>39</v>
       </c>
     </row>
   </sheetData>
@@ -4804,30 +5176,30 @@
     <mergeCell ref="Z3:AC3"/>
     <mergeCell ref="AD3:AG3"/>
     <mergeCell ref="A5:AK5"/>
-    <mergeCell ref="A19:AK19"/>
-    <mergeCell ref="B34:AK34"/>
-    <mergeCell ref="B35:E35"/>
-    <mergeCell ref="F35:AG35"/>
-    <mergeCell ref="B36:E36"/>
-    <mergeCell ref="F36:I36"/>
-    <mergeCell ref="J36:M36"/>
-    <mergeCell ref="N36:Q36"/>
-    <mergeCell ref="R36:U36"/>
-    <mergeCell ref="V36:Y36"/>
-    <mergeCell ref="Z36:AC36"/>
-    <mergeCell ref="AD36:AG36"/>
-    <mergeCell ref="A38:AK38"/>
-    <mergeCell ref="A48:AK48"/>
+    <mergeCell ref="A21:AK21"/>
+    <mergeCell ref="B36:AK36"/>
+    <mergeCell ref="B37:E37"/>
+    <mergeCell ref="F37:AG37"/>
+    <mergeCell ref="B38:E38"/>
+    <mergeCell ref="F38:I38"/>
+    <mergeCell ref="J38:M38"/>
+    <mergeCell ref="N38:Q38"/>
+    <mergeCell ref="R38:U38"/>
+    <mergeCell ref="V38:Y38"/>
+    <mergeCell ref="Z38:AC38"/>
+    <mergeCell ref="AD38:AG38"/>
+    <mergeCell ref="A40:AK40"/>
+    <mergeCell ref="A50:AK50"/>
     <mergeCell ref="A1:A4"/>
-    <mergeCell ref="A34:A37"/>
+    <mergeCell ref="A36:A39"/>
     <mergeCell ref="AH2:AH4"/>
-    <mergeCell ref="AH35:AH37"/>
+    <mergeCell ref="AH37:AH39"/>
     <mergeCell ref="AI2:AI4"/>
-    <mergeCell ref="AI35:AI37"/>
+    <mergeCell ref="AI37:AI39"/>
     <mergeCell ref="AJ2:AJ4"/>
-    <mergeCell ref="AJ35:AJ37"/>
+    <mergeCell ref="AJ37:AJ39"/>
     <mergeCell ref="AK2:AK4"/>
-    <mergeCell ref="AK35:AK37"/>
+    <mergeCell ref="AK37:AK39"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter/>

</xml_diff>